<commit_message>
ZK Spreadsheet App: code fine-tune
</commit_message>
<xml_diff>
--- a/trunk/zssapp/WebContent/xls/ZSS-demo_sample.xlsx
+++ b/trunk/zssapp/WebContent/xls/ZSS-demo_sample.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Assets!$A$1:$Z$30</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">Debt!$A$1:$Z$29</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Input!$A$1:$J$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Input!$A$1:$J$38</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Liquidity!$A$1:$AJ$58</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">Market!$A$1:$Z$30</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">Profitability!$A$1:$Z$52</definedName>
@@ -1402,16 +1402,16 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -1533,7 +1533,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Input!$J$14,Input!$J$20,Input!$J$21)</c:f>
+              <c:f>(Input!$J$15,Input!$J$21,Input!$J$22)</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1565,7 +1565,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.7330779054916986"/>
-          <c:y val="0.30801248699271605"/>
+          <c:y val="0.30801248699271616"/>
           <c:w val="0.23499361430395913"/>
           <c:h val="0.37044745057232054"/>
         </c:manualLayout>
@@ -1576,7 +1576,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1594,7 +1594,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>922020</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1908,10 +1908,10 @@
     <tabColor indexed="12"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
@@ -1943,7 +1943,7 @@
     </row>
     <row r="2" spans="1:11" ht="6" customHeight="1">
       <c r="A2" s="14"/>
-      <c r="B2" s="18"/>
+      <c r="B2" s="15"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
       <c r="E2" s="16"/>
@@ -1952,301 +1952,288 @@
       <c r="H2" s="16"/>
       <c r="I2" s="16"/>
       <c r="J2" s="14"/>
-      <c r="K2" s="17"/>
-    </row>
-    <row r="3" spans="1:11" ht="30" customHeight="1">
+      <c r="K2" s="14"/>
+    </row>
+    <row r="3" spans="1:11" ht="6" customHeight="1">
       <c r="A3" s="14"/>
-      <c r="B3" s="197" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="17"/>
+    </row>
+    <row r="4" spans="1:11" ht="30" customHeight="1">
+      <c r="A4" s="14"/>
+      <c r="B4" s="197" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="198"/>
-      <c r="D3" s="198"/>
-      <c r="E3" s="198"/>
-      <c r="F3" s="198"/>
-      <c r="G3" s="198"/>
-      <c r="H3" s="198"/>
-      <c r="I3" s="198"/>
-      <c r="J3" s="198"/>
-      <c r="K3" s="17"/>
-    </row>
-    <row r="4" spans="1:11" ht="6" customHeight="1">
-      <c r="A4" s="14"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="14"/>
+      <c r="C4" s="198"/>
+      <c r="D4" s="198"/>
+      <c r="E4" s="198"/>
+      <c r="F4" s="198"/>
+      <c r="G4" s="198"/>
+      <c r="H4" s="198"/>
+      <c r="I4" s="198"/>
+      <c r="J4" s="198"/>
       <c r="K4" s="17"/>
     </row>
-    <row r="5" spans="1:11" ht="30.75" customHeight="1">
+    <row r="5" spans="1:11" ht="6" customHeight="1">
       <c r="A5" s="14"/>
-      <c r="B5" s="196" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="17"/>
+    </row>
+    <row r="6" spans="1:11" ht="30.75" customHeight="1">
+      <c r="A6" s="14"/>
+      <c r="B6" s="196" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="196"/>
-      <c r="D5" s="196"/>
-      <c r="E5" s="196"/>
-      <c r="F5" s="183" t="s">
+      <c r="C6" s="196"/>
+      <c r="D6" s="196"/>
+      <c r="E6" s="196"/>
+      <c r="F6" s="183" t="s">
         <v>69</v>
-      </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="17"/>
-    </row>
-    <row r="6" spans="1:11" ht="14.4">
-      <c r="A6" s="14"/>
-      <c r="B6" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="24">
-        <v>12500</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
-      <c r="I6" s="148"/>
+      <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="17"/>
     </row>
     <row r="7" spans="1:11" ht="14.4">
       <c r="A7" s="14"/>
-      <c r="B7" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="28">
-        <v>120000</v>
+      <c r="B7" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="24">
+        <v>12500</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
+      <c r="I7" s="148"/>
       <c r="J7" s="20"/>
       <c r="K7" s="17"/>
     </row>
     <row r="8" spans="1:11" ht="14.4">
       <c r="A8" s="14"/>
       <c r="B8" s="25" t="s">
-        <v>97</v>
+        <v>46</v>
       </c>
       <c r="C8" s="26"/>
       <c r="D8" s="26"/>
       <c r="E8" s="27"/>
       <c r="F8" s="28">
-        <v>29000</v>
+        <v>120000</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
-      <c r="I8" s="19"/>
+      <c r="I8" s="20"/>
       <c r="J8" s="20"/>
       <c r="K8" s="17"/>
     </row>
     <row r="9" spans="1:11" ht="14.4">
       <c r="A9" s="14"/>
-      <c r="B9" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="32">
-        <v>25000</v>
+      <c r="B9" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="28">
+        <v>29000</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
+      <c r="I9" s="19"/>
       <c r="J9" s="20"/>
       <c r="K9" s="17"/>
     </row>
-    <row r="10" spans="1:11" s="10" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A10" s="33"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-    </row>
-    <row r="11" spans="1:11" s="11" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A11" s="35"/>
-      <c r="B11" s="196" t="s">
+    <row r="10" spans="1:11" ht="14.4">
+      <c r="A10" s="14"/>
+      <c r="B10" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="32">
+        <v>25000</v>
+      </c>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="17"/>
+    </row>
+    <row r="11" spans="1:11" s="10" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A11" s="33"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+    </row>
+    <row r="12" spans="1:11" s="11" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A12" s="35"/>
+      <c r="B12" s="196" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="196"/>
-      <c r="D11" s="196"/>
-      <c r="E11" s="196"/>
-      <c r="F11" s="181" t="s">
+      <c r="C12" s="196"/>
+      <c r="D12" s="196"/>
+      <c r="E12" s="196"/>
+      <c r="F12" s="181" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="181" t="s">
+      <c r="G12" s="181" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="181" t="s">
+      <c r="H12" s="181" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="181" t="s">
+      <c r="I12" s="181" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="181" t="s">
+      <c r="J12" s="181" t="s">
         <v>35</v>
       </c>
-      <c r="K11" s="35"/>
-    </row>
-    <row r="12" spans="1:11" ht="14.4">
-      <c r="A12" s="14"/>
-      <c r="B12" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="36">
-        <v>45000</v>
-      </c>
-      <c r="G12" s="36">
-        <v>46000</v>
-      </c>
-      <c r="H12" s="36">
-        <v>46500</v>
-      </c>
-      <c r="I12" s="37">
-        <v>56000</v>
-      </c>
-      <c r="J12" s="182">
-        <f>+I12</f>
-        <v>56000</v>
-      </c>
-      <c r="K12" s="14"/>
+      <c r="K12" s="35"/>
     </row>
     <row r="13" spans="1:11" ht="14.4">
       <c r="A13" s="14"/>
-      <c r="B13" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="38">
-        <v>80000</v>
-      </c>
-      <c r="G13" s="38">
-        <v>80000</v>
-      </c>
-      <c r="H13" s="38">
-        <v>80000</v>
-      </c>
-      <c r="I13" s="39">
-        <v>80000</v>
-      </c>
-      <c r="J13" s="186">
+      <c r="B13" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="36">
+        <v>45000</v>
+      </c>
+      <c r="G13" s="36">
+        <v>46000</v>
+      </c>
+      <c r="H13" s="36">
+        <v>46500</v>
+      </c>
+      <c r="I13" s="37">
+        <v>56000</v>
+      </c>
+      <c r="J13" s="182">
         <f>+I13</f>
-        <v>80000</v>
+        <v>56000</v>
       </c>
       <c r="K13" s="14"/>
     </row>
     <row r="14" spans="1:11" ht="14.4">
       <c r="A14" s="14"/>
       <c r="B14" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="26"/>
       <c r="D14" s="26"/>
       <c r="E14" s="27"/>
-      <c r="F14" s="184">
-        <f>F12+F13</f>
-        <v>125000</v>
-      </c>
-      <c r="G14" s="184">
-        <f>G12+G13</f>
-        <v>126000</v>
-      </c>
-      <c r="H14" s="184">
-        <f>H12+H13</f>
-        <v>126500</v>
-      </c>
-      <c r="I14" s="184">
-        <f>I12+I13</f>
-        <v>136000</v>
-      </c>
-      <c r="J14" s="185">
-        <f>I14</f>
-        <v>136000</v>
+      <c r="F14" s="38">
+        <v>80000</v>
+      </c>
+      <c r="G14" s="38">
+        <v>80000</v>
+      </c>
+      <c r="H14" s="38">
+        <v>80000</v>
+      </c>
+      <c r="I14" s="39">
+        <v>80000</v>
+      </c>
+      <c r="J14" s="186">
+        <f>+I14</f>
+        <v>80000</v>
       </c>
       <c r="K14" s="14"/>
     </row>
     <row r="15" spans="1:11" ht="14.4">
       <c r="A15" s="14"/>
       <c r="B15" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="26"/>
       <c r="D15" s="26"/>
       <c r="E15" s="27"/>
       <c r="F15" s="184">
-        <f>AVERAGE($F$7,F14)</f>
-        <v>122500</v>
+        <f>F13+F14</f>
+        <v>125000</v>
       </c>
       <c r="G15" s="184">
-        <f>AVERAGE($F$7,G14)</f>
-        <v>123000</v>
+        <f>G13+G14</f>
+        <v>126000</v>
       </c>
       <c r="H15" s="184">
-        <f>AVERAGE($F$7,H14)</f>
-        <v>123250</v>
+        <f>H13+H14</f>
+        <v>126500</v>
       </c>
       <c r="I15" s="184">
-        <f>AVERAGE($F$7,I14)</f>
-        <v>128000</v>
+        <f>I13+I14</f>
+        <v>136000</v>
       </c>
       <c r="J15" s="185">
-        <f t="shared" ref="J15:J24" si="0">I15</f>
-        <v>128000</v>
+        <f>I15</f>
+        <v>136000</v>
       </c>
       <c r="K15" s="14"/>
     </row>
     <row r="16" spans="1:11" ht="14.4">
       <c r="A16" s="14"/>
       <c r="B16" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="26"/>
       <c r="D16" s="26"/>
       <c r="E16" s="27"/>
-      <c r="F16" s="38">
-        <v>15000</v>
-      </c>
-      <c r="G16" s="38">
-        <v>18000</v>
-      </c>
-      <c r="H16" s="38">
-        <v>16500</v>
-      </c>
-      <c r="I16" s="39">
-        <v>14350</v>
+      <c r="F16" s="184">
+        <f>AVERAGE($F$8,F15)</f>
+        <v>122500</v>
+      </c>
+      <c r="G16" s="184">
+        <f>AVERAGE($F$8,G15)</f>
+        <v>123000</v>
+      </c>
+      <c r="H16" s="184">
+        <f>AVERAGE($F$8,H15)</f>
+        <v>123250</v>
+      </c>
+      <c r="I16" s="184">
+        <f>AVERAGE($F$8,I15)</f>
+        <v>128000</v>
       </c>
       <c r="J16" s="185">
-        <f t="shared" si="0"/>
-        <v>14350</v>
+        <f t="shared" ref="J16:J25" si="0">I16</f>
+        <v>128000</v>
       </c>
       <c r="K16" s="14"/>
     </row>
     <row r="17" spans="1:11" ht="14.4">
       <c r="A17" s="14"/>
       <c r="B17" s="25" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="C17" s="26"/>
       <c r="D17" s="26"/>
@@ -2272,159 +2259,155 @@
     <row r="18" spans="1:11" ht="14.4">
       <c r="A18" s="14"/>
       <c r="B18" s="25" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C18" s="26"/>
       <c r="D18" s="26"/>
       <c r="E18" s="27"/>
-      <c r="F18" s="184">
-        <f>AVERAGE($F$6,F17)</f>
-        <v>13750</v>
-      </c>
-      <c r="G18" s="184">
-        <f>AVERAGE($F$6,G17)</f>
-        <v>15250</v>
-      </c>
-      <c r="H18" s="184">
-        <f>AVERAGE($F$6,H17)</f>
-        <v>14500</v>
-      </c>
-      <c r="I18" s="184">
-        <f>AVERAGE($F$6,I17)</f>
-        <v>13425</v>
+      <c r="F18" s="38">
+        <v>15000</v>
+      </c>
+      <c r="G18" s="38">
+        <v>18000</v>
+      </c>
+      <c r="H18" s="38">
+        <v>16500</v>
+      </c>
+      <c r="I18" s="39">
+        <v>14350</v>
       </c>
       <c r="J18" s="185">
         <f t="shared" si="0"/>
-        <v>13425</v>
+        <v>14350</v>
       </c>
       <c r="K18" s="14"/>
     </row>
     <row r="19" spans="1:11" ht="14.4">
       <c r="A19" s="14"/>
       <c r="B19" s="25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
       <c r="E19" s="27"/>
-      <c r="F19" s="38">
-        <v>23000</v>
-      </c>
-      <c r="G19" s="38">
-        <v>25000</v>
-      </c>
-      <c r="H19" s="38">
-        <v>22500</v>
-      </c>
-      <c r="I19" s="39">
-        <v>25600</v>
+      <c r="F19" s="184">
+        <f>AVERAGE($F$7,F18)</f>
+        <v>13750</v>
+      </c>
+      <c r="G19" s="184">
+        <f>AVERAGE($F$7,G18)</f>
+        <v>15250</v>
+      </c>
+      <c r="H19" s="184">
+        <f>AVERAGE($F$7,H18)</f>
+        <v>14500</v>
+      </c>
+      <c r="I19" s="184">
+        <f>AVERAGE($F$7,I18)</f>
+        <v>13425</v>
       </c>
       <c r="J19" s="185">
         <f t="shared" si="0"/>
-        <v>25600</v>
+        <v>13425</v>
       </c>
       <c r="K19" s="14"/>
     </row>
     <row r="20" spans="1:11" ht="14.4">
       <c r="A20" s="14"/>
       <c r="B20" s="25" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
       <c r="E20" s="27"/>
       <c r="F20" s="38">
-        <v>125000</v>
+        <v>23000</v>
       </c>
       <c r="G20" s="38">
-        <v>125000</v>
+        <v>25000</v>
       </c>
       <c r="H20" s="38">
-        <v>125000</v>
+        <v>22500</v>
       </c>
       <c r="I20" s="39">
-        <v>110000</v>
+        <v>25600</v>
       </c>
       <c r="J20" s="185">
         <f t="shared" si="0"/>
-        <v>110000</v>
+        <v>25600</v>
       </c>
       <c r="K20" s="14"/>
     </row>
     <row r="21" spans="1:11" ht="14.4">
       <c r="A21" s="14"/>
       <c r="B21" s="25" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
       <c r="E21" s="27"/>
       <c r="F21" s="38">
-        <v>28000</v>
+        <v>125000</v>
       </c>
       <c r="G21" s="38">
-        <v>30900</v>
+        <v>125000</v>
       </c>
       <c r="H21" s="38">
-        <v>32000</v>
+        <v>125000</v>
       </c>
       <c r="I21" s="39">
-        <v>26000</v>
+        <v>110000</v>
       </c>
       <c r="J21" s="185">
         <f t="shared" si="0"/>
-        <v>26000</v>
+        <v>110000</v>
       </c>
       <c r="K21" s="14"/>
     </row>
     <row r="22" spans="1:11" ht="14.4">
       <c r="A22" s="14"/>
       <c r="B22" s="25" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="C22" s="26"/>
       <c r="D22" s="26"/>
       <c r="E22" s="27"/>
       <c r="F22" s="38">
-        <v>25000</v>
+        <v>28000</v>
       </c>
       <c r="G22" s="38">
-        <v>25000</v>
+        <v>30900</v>
       </c>
       <c r="H22" s="38">
-        <v>25000</v>
+        <v>32000</v>
       </c>
       <c r="I22" s="39">
-        <v>25000</v>
-      </c>
-      <c r="J22" s="184">
+        <v>26000</v>
+      </c>
+      <c r="J22" s="185">
         <f t="shared" si="0"/>
-        <v>25000</v>
+        <v>26000</v>
       </c>
       <c r="K22" s="14"/>
     </row>
     <row r="23" spans="1:11" ht="14.4">
       <c r="A23" s="14"/>
       <c r="B23" s="25" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C23" s="26"/>
       <c r="D23" s="26"/>
       <c r="E23" s="27"/>
-      <c r="F23" s="184">
-        <f>AVERAGE($F$9,F22)</f>
+      <c r="F23" s="38">
         <v>25000</v>
       </c>
-      <c r="G23" s="184">
-        <f>AVERAGE($F$9,G22)</f>
+      <c r="G23" s="38">
         <v>25000</v>
       </c>
-      <c r="H23" s="184">
-        <f>AVERAGE($F$9,H22)</f>
+      <c r="H23" s="38">
         <v>25000</v>
       </c>
-      <c r="I23" s="184">
-        <f>AVERAGE($F$9,I22)</f>
+      <c r="I23" s="39">
         <v>25000</v>
       </c>
       <c r="J23" s="184">
@@ -2436,442 +2419,459 @@
     <row r="24" spans="1:11" ht="14.4">
       <c r="A24" s="14"/>
       <c r="B24" s="25" t="s">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="C24" s="26"/>
       <c r="D24" s="26"/>
       <c r="E24" s="27"/>
       <c r="F24" s="184">
-        <f>AVERAGE($F$8,F21)</f>
-        <v>28500</v>
+        <f>AVERAGE($F$10,F23)</f>
+        <v>25000</v>
       </c>
       <c r="G24" s="184">
-        <f>AVERAGE($F$8,G21)</f>
-        <v>29950</v>
+        <f>AVERAGE($F$10,G23)</f>
+        <v>25000</v>
       </c>
       <c r="H24" s="184">
-        <f>AVERAGE($F$8,H21)</f>
-        <v>30500</v>
+        <f>AVERAGE($F$10,H23)</f>
+        <v>25000</v>
       </c>
       <c r="I24" s="184">
-        <f>AVERAGE($F$8,I21)</f>
-        <v>27500</v>
-      </c>
-      <c r="J24" s="185">
+        <f>AVERAGE($F$10,I23)</f>
+        <v>25000</v>
+      </c>
+      <c r="J24" s="184">
         <f t="shared" si="0"/>
-        <v>27500</v>
+        <v>25000</v>
       </c>
       <c r="K24" s="14"/>
     </row>
     <row r="25" spans="1:11" ht="14.4">
       <c r="A25" s="14"/>
       <c r="B25" s="25" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="C25" s="26"/>
       <c r="D25" s="26"/>
       <c r="E25" s="27"/>
-      <c r="F25" s="40">
-        <v>10</v>
-      </c>
-      <c r="G25" s="40">
-        <v>10</v>
-      </c>
-      <c r="H25" s="40">
-        <v>10</v>
-      </c>
-      <c r="I25" s="41">
-        <v>10</v>
-      </c>
-      <c r="J25" s="187">
-        <f>+I25</f>
-        <v>10</v>
+      <c r="F25" s="184">
+        <f>AVERAGE($F$9,F22)</f>
+        <v>28500</v>
+      </c>
+      <c r="G25" s="184">
+        <f>AVERAGE($F$9,G22)</f>
+        <v>29950</v>
+      </c>
+      <c r="H25" s="184">
+        <f>AVERAGE($F$9,H22)</f>
+        <v>30500</v>
+      </c>
+      <c r="I25" s="184">
+        <f>AVERAGE($F$9,I22)</f>
+        <v>27500</v>
+      </c>
+      <c r="J25" s="185">
+        <f t="shared" si="0"/>
+        <v>27500</v>
       </c>
       <c r="K25" s="14"/>
     </row>
     <row r="26" spans="1:11" ht="14.4">
       <c r="A26" s="14"/>
       <c r="B26" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
       <c r="E26" s="27"/>
-      <c r="F26" s="38">
-        <v>175000</v>
-      </c>
-      <c r="G26" s="38">
-        <v>186000</v>
-      </c>
-      <c r="H26" s="38">
-        <v>169000</v>
-      </c>
-      <c r="I26" s="39">
-        <v>155000</v>
-      </c>
-      <c r="J26" s="186">
-        <f>SUM(F26:I26)</f>
-        <v>685000</v>
+      <c r="F26" s="40">
+        <v>10</v>
+      </c>
+      <c r="G26" s="40">
+        <v>10</v>
+      </c>
+      <c r="H26" s="40">
+        <v>10</v>
+      </c>
+      <c r="I26" s="41">
+        <v>10</v>
+      </c>
+      <c r="J26" s="187">
+        <f>+I26</f>
+        <v>10</v>
       </c>
       <c r="K26" s="14"/>
     </row>
     <row r="27" spans="1:11" ht="14.4">
       <c r="A27" s="14"/>
       <c r="B27" s="25" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
       <c r="E27" s="27"/>
-      <c r="F27" s="189">
-        <f>F26/F23</f>
-        <v>7</v>
-      </c>
-      <c r="G27" s="189">
-        <f>G26/G23</f>
-        <v>7.44</v>
-      </c>
-      <c r="H27" s="189">
-        <f>H26/H23</f>
-        <v>6.76</v>
-      </c>
-      <c r="I27" s="189">
-        <f>I26/I23</f>
-        <v>6.2</v>
-      </c>
-      <c r="J27" s="188">
-        <f>J26/J23</f>
-        <v>27.4</v>
+      <c r="F27" s="38">
+        <v>175000</v>
+      </c>
+      <c r="G27" s="38">
+        <v>186000</v>
+      </c>
+      <c r="H27" s="38">
+        <v>169000</v>
+      </c>
+      <c r="I27" s="39">
+        <v>155000</v>
+      </c>
+      <c r="J27" s="186">
+        <f>SUM(F27:I27)</f>
+        <v>685000</v>
       </c>
       <c r="K27" s="14"/>
     </row>
     <row r="28" spans="1:11" ht="14.4">
       <c r="A28" s="14"/>
       <c r="B28" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
       <c r="E28" s="27"/>
-      <c r="F28" s="38">
-        <v>5000</v>
-      </c>
-      <c r="G28" s="38">
-        <v>5000</v>
-      </c>
-      <c r="H28" s="38">
-        <v>5000</v>
-      </c>
-      <c r="I28" s="39">
-        <v>5000</v>
-      </c>
-      <c r="J28" s="186">
-        <f>SUM(F28:I28)</f>
-        <v>20000</v>
+      <c r="F28" s="189">
+        <f>F27/F24</f>
+        <v>7</v>
+      </c>
+      <c r="G28" s="189">
+        <f>G27/G24</f>
+        <v>7.44</v>
+      </c>
+      <c r="H28" s="189">
+        <f>H27/H24</f>
+        <v>6.76</v>
+      </c>
+      <c r="I28" s="189">
+        <f>I27/I24</f>
+        <v>6.2</v>
+      </c>
+      <c r="J28" s="188">
+        <f>J27/J24</f>
+        <v>27.4</v>
       </c>
       <c r="K28" s="14"/>
     </row>
     <row r="29" spans="1:11" ht="14.4">
       <c r="A29" s="14"/>
-      <c r="B29" s="42"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="47"/>
+      <c r="B29" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="38">
+        <v>5000</v>
+      </c>
+      <c r="G29" s="38">
+        <v>5000</v>
+      </c>
+      <c r="H29" s="38">
+        <v>5000</v>
+      </c>
+      <c r="I29" s="39">
+        <v>5000</v>
+      </c>
+      <c r="J29" s="186">
+        <f>SUM(F29:I29)</f>
+        <v>20000</v>
+      </c>
       <c r="K29" s="14"/>
     </row>
     <row r="30" spans="1:11" ht="14.4">
       <c r="A30" s="14"/>
-      <c r="B30" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="51">
-        <v>145000</v>
-      </c>
-      <c r="G30" s="51">
-        <v>156000</v>
-      </c>
-      <c r="H30" s="51">
-        <v>135600</v>
-      </c>
-      <c r="I30" s="52">
-        <v>125000</v>
-      </c>
-      <c r="J30" s="186">
-        <f t="shared" ref="J30:J37" si="1">SUM(F30:I30)</f>
-        <v>561600</v>
-      </c>
+      <c r="B30" s="42"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="47"/>
       <c r="K30" s="14"/>
     </row>
     <row r="31" spans="1:11" ht="14.4">
       <c r="A31" s="14"/>
-      <c r="B31" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="38">
-        <v>68000</v>
-      </c>
-      <c r="G31" s="38">
-        <v>68000</v>
-      </c>
-      <c r="H31" s="38">
-        <v>68000</v>
-      </c>
-      <c r="I31" s="39">
-        <v>68000</v>
+      <c r="B31" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="51">
+        <v>145000</v>
+      </c>
+      <c r="G31" s="51">
+        <v>156000</v>
+      </c>
+      <c r="H31" s="51">
+        <v>135600</v>
+      </c>
+      <c r="I31" s="52">
+        <v>125000</v>
       </c>
       <c r="J31" s="186">
-        <f t="shared" si="1"/>
-        <v>272000</v>
+        <f t="shared" ref="J31:J38" si="1">SUM(F31:I31)</f>
+        <v>561600</v>
       </c>
       <c r="K31" s="14"/>
     </row>
     <row r="32" spans="1:11" ht="14.4">
       <c r="A32" s="14"/>
       <c r="B32" s="25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C32" s="26"/>
       <c r="D32" s="26"/>
       <c r="E32" s="27"/>
-      <c r="F32" s="184">
-        <f>F30-F31</f>
-        <v>77000</v>
-      </c>
-      <c r="G32" s="184">
-        <f>G30-G31</f>
-        <v>88000</v>
-      </c>
-      <c r="H32" s="184">
-        <f>H30-H31</f>
-        <v>67600</v>
-      </c>
-      <c r="I32" s="184">
-        <f>I30-I31</f>
-        <v>57000</v>
+      <c r="F32" s="38">
+        <v>68000</v>
+      </c>
+      <c r="G32" s="38">
+        <v>68000</v>
+      </c>
+      <c r="H32" s="38">
+        <v>68000</v>
+      </c>
+      <c r="I32" s="39">
+        <v>68000</v>
       </c>
       <c r="J32" s="186">
         <f t="shared" si="1"/>
-        <v>289600</v>
+        <v>272000</v>
       </c>
       <c r="K32" s="14"/>
     </row>
     <row r="33" spans="1:11" ht="14.4">
       <c r="A33" s="14"/>
       <c r="B33" s="25" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="C33" s="26"/>
       <c r="D33" s="26"/>
       <c r="E33" s="27"/>
-      <c r="F33" s="38">
-        <v>18000</v>
-      </c>
-      <c r="G33" s="38">
-        <v>18000</v>
-      </c>
-      <c r="H33" s="38">
-        <v>18000</v>
-      </c>
-      <c r="I33" s="39">
-        <v>18000</v>
+      <c r="F33" s="184">
+        <f>F31-F32</f>
+        <v>77000</v>
+      </c>
+      <c r="G33" s="184">
+        <f>G31-G32</f>
+        <v>88000</v>
+      </c>
+      <c r="H33" s="184">
+        <f>H31-H32</f>
+        <v>67600</v>
+      </c>
+      <c r="I33" s="184">
+        <f>I31-I32</f>
+        <v>57000</v>
       </c>
       <c r="J33" s="186">
         <f t="shared" si="1"/>
-        <v>72000</v>
+        <v>289600</v>
       </c>
       <c r="K33" s="14"/>
     </row>
     <row r="34" spans="1:11" ht="14.4">
       <c r="A34" s="14"/>
       <c r="B34" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C34" s="26"/>
       <c r="D34" s="26"/>
       <c r="E34" s="27"/>
       <c r="F34" s="38">
-        <v>11000</v>
+        <v>18000</v>
       </c>
       <c r="G34" s="38">
-        <v>11000</v>
+        <v>18000</v>
       </c>
       <c r="H34" s="38">
-        <v>11000</v>
+        <v>18000</v>
       </c>
       <c r="I34" s="39">
-        <v>11000</v>
+        <v>18000</v>
       </c>
       <c r="J34" s="186">
         <f t="shared" si="1"/>
-        <v>44000</v>
+        <v>72000</v>
       </c>
       <c r="K34" s="14"/>
     </row>
     <row r="35" spans="1:11" ht="14.4">
       <c r="A35" s="14"/>
       <c r="B35" s="25" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="C35" s="26"/>
       <c r="D35" s="26"/>
       <c r="E35" s="27"/>
       <c r="F35" s="38">
-        <v>132000</v>
+        <v>11000</v>
       </c>
       <c r="G35" s="38">
-        <v>127000</v>
+        <v>11000</v>
       </c>
       <c r="H35" s="38">
-        <v>114500</v>
+        <v>11000</v>
       </c>
       <c r="I35" s="39">
-        <v>98000</v>
+        <v>11000</v>
       </c>
       <c r="J35" s="186">
         <f t="shared" si="1"/>
-        <v>471500</v>
+        <v>44000</v>
       </c>
       <c r="K35" s="14"/>
     </row>
     <row r="36" spans="1:11" ht="14.4">
       <c r="A36" s="14"/>
       <c r="B36" s="25" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C36" s="26"/>
       <c r="D36" s="26"/>
       <c r="E36" s="27"/>
       <c r="F36" s="38">
-        <v>24000</v>
+        <v>132000</v>
       </c>
       <c r="G36" s="38">
-        <v>24000</v>
+        <v>127000</v>
       </c>
       <c r="H36" s="38">
-        <v>24000</v>
+        <v>114500</v>
       </c>
       <c r="I36" s="39">
-        <v>24000</v>
+        <v>98000</v>
       </c>
       <c r="J36" s="186">
         <f t="shared" si="1"/>
-        <v>96000</v>
+        <v>471500</v>
       </c>
       <c r="K36" s="14"/>
     </row>
     <row r="37" spans="1:11" ht="14.4">
       <c r="A37" s="14"/>
       <c r="B37" s="25" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C37" s="26"/>
       <c r="D37" s="26"/>
       <c r="E37" s="27"/>
       <c r="F37" s="38">
-        <v>89000</v>
+        <v>24000</v>
       </c>
       <c r="G37" s="38">
-        <v>87000</v>
+        <v>24000</v>
       </c>
       <c r="H37" s="38">
-        <v>95000</v>
+        <v>24000</v>
       </c>
       <c r="I37" s="39">
-        <v>65000</v>
+        <v>24000</v>
       </c>
       <c r="J37" s="186">
         <f t="shared" si="1"/>
+        <v>96000</v>
+      </c>
+      <c r="K37" s="14"/>
+    </row>
+    <row r="38" spans="1:11" ht="14.4">
+      <c r="A38" s="14"/>
+      <c r="B38" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="38">
+        <v>89000</v>
+      </c>
+      <c r="G38" s="38">
+        <v>87000</v>
+      </c>
+      <c r="H38" s="38">
+        <v>95000</v>
+      </c>
+      <c r="I38" s="39">
+        <v>65000</v>
+      </c>
+      <c r="J38" s="186">
+        <f t="shared" si="1"/>
         <v>336000</v>
       </c>
-      <c r="K37" s="14"/>
-    </row>
-    <row r="38" spans="1:11">
-      <c r="A38" s="14"/>
-      <c r="B38" s="53"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="54"/>
-      <c r="F38" s="55"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="55"/>
-      <c r="J38" s="56"/>
       <c r="K38" s="14"/>
     </row>
-    <row r="39" spans="1:11" ht="14.4">
+    <row r="39" spans="1:11">
       <c r="A39" s="14"/>
-      <c r="B39" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="38">
-        <v>25000</v>
-      </c>
-      <c r="G39" s="38">
-        <v>24000</v>
-      </c>
-      <c r="H39" s="38">
-        <v>23000</v>
-      </c>
-      <c r="I39" s="39">
-        <v>22000</v>
-      </c>
-      <c r="J39" s="186">
-        <f>+I39</f>
-        <v>22000</v>
-      </c>
+      <c r="B39" s="53"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="55"/>
+      <c r="G39" s="55"/>
+      <c r="H39" s="55"/>
+      <c r="I39" s="55"/>
+      <c r="J39" s="56"/>
       <c r="K39" s="14"/>
     </row>
     <row r="40" spans="1:11" ht="14.4">
       <c r="A40" s="14"/>
-      <c r="B40" s="29" t="s">
+      <c r="B40" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="38">
+        <v>25000</v>
+      </c>
+      <c r="G40" s="38">
+        <v>24000</v>
+      </c>
+      <c r="H40" s="38">
+        <v>23000</v>
+      </c>
+      <c r="I40" s="39">
+        <v>22000</v>
+      </c>
+      <c r="J40" s="186">
+        <f>+I40</f>
+        <v>22000</v>
+      </c>
+      <c r="K40" s="14"/>
+    </row>
+    <row r="41" spans="1:11" ht="14.4">
+      <c r="A41" s="14"/>
+      <c r="B41" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="32">
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="32">
         <v>65000</v>
       </c>
-      <c r="G40" s="32">
+      <c r="G41" s="32">
         <v>65000</v>
       </c>
-      <c r="H40" s="32">
+      <c r="H41" s="32">
         <v>65000</v>
       </c>
-      <c r="I40" s="57">
+      <c r="I41" s="57">
         <v>65000</v>
       </c>
-      <c r="J40" s="190">
-        <f>+I40</f>
+      <c r="J41" s="190">
+        <f>+I41</f>
         <v>65000</v>
       </c>
-      <c r="K40" s="14"/>
-    </row>
-    <row r="41" spans="1:11">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
-      <c r="I41" s="16"/>
-      <c r="J41" s="14"/>
       <c r="K41" s="14"/>
     </row>
     <row r="42" spans="1:11">
@@ -2887,11 +2887,24 @@
       <c r="J42" s="14"/>
       <c r="K42" s="14"/>
     </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="14"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="14"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B4:J4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -2899,7 +2912,7 @@
   <pageSetup scale="80" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="J27" formula="1"/>
+    <ignoredError sqref="J28" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -3045,48 +3058,48 @@
       <c r="D3" s="195"/>
       <c r="E3" s="195"/>
       <c r="F3" s="195"/>
-      <c r="G3" s="199" t="s">
+      <c r="G3" s="201" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="200"/>
-      <c r="I3" s="200"/>
-      <c r="J3" s="200"/>
-      <c r="K3" s="200"/>
-      <c r="L3" s="200"/>
-      <c r="M3" s="199" t="s">
+      <c r="H3" s="202"/>
+      <c r="I3" s="202"/>
+      <c r="J3" s="202"/>
+      <c r="K3" s="202"/>
+      <c r="L3" s="202"/>
+      <c r="M3" s="201" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="200"/>
-      <c r="O3" s="200"/>
-      <c r="P3" s="200" t="s">
+      <c r="N3" s="202"/>
+      <c r="O3" s="202"/>
+      <c r="P3" s="202" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" s="200"/>
-      <c r="R3" s="200"/>
-      <c r="S3" s="199" t="s">
+      <c r="Q3" s="202"/>
+      <c r="R3" s="202"/>
+      <c r="S3" s="201" t="s">
         <v>33</v>
       </c>
-      <c r="T3" s="200"/>
-      <c r="U3" s="200"/>
-      <c r="V3" s="200"/>
-      <c r="W3" s="200"/>
-      <c r="X3" s="200"/>
-      <c r="Y3" s="199" t="s">
+      <c r="T3" s="202"/>
+      <c r="U3" s="202"/>
+      <c r="V3" s="202"/>
+      <c r="W3" s="202"/>
+      <c r="X3" s="202"/>
+      <c r="Y3" s="201" t="s">
         <v>34</v>
       </c>
-      <c r="Z3" s="200"/>
-      <c r="AA3" s="200"/>
-      <c r="AB3" s="200"/>
-      <c r="AC3" s="200"/>
-      <c r="AD3" s="200"/>
-      <c r="AE3" s="199" t="s">
+      <c r="Z3" s="202"/>
+      <c r="AA3" s="202"/>
+      <c r="AB3" s="202"/>
+      <c r="AC3" s="202"/>
+      <c r="AD3" s="202"/>
+      <c r="AE3" s="201" t="s">
         <v>35</v>
       </c>
-      <c r="AF3" s="200"/>
-      <c r="AG3" s="200"/>
-      <c r="AH3" s="200"/>
-      <c r="AI3" s="200"/>
-      <c r="AJ3" s="200"/>
+      <c r="AF3" s="202"/>
+      <c r="AG3" s="202"/>
+      <c r="AH3" s="202"/>
+      <c r="AI3" s="202"/>
+      <c r="AJ3" s="202"/>
     </row>
     <row r="4" spans="1:37">
       <c r="A4" s="62"/>
@@ -3190,7 +3203,7 @@
         <v>7</v>
       </c>
       <c r="J6" s="192">
-        <f>Input!F12</f>
+        <f>Input!F13</f>
         <v>45000</v>
       </c>
       <c r="K6" s="68"/>
@@ -3204,7 +3217,7 @@
         <v>7</v>
       </c>
       <c r="P6" s="192">
-        <f>Input!G12</f>
+        <f>Input!G13</f>
         <v>46000</v>
       </c>
       <c r="Q6" s="68"/>
@@ -3218,7 +3231,7 @@
         <v>7</v>
       </c>
       <c r="V6" s="192">
-        <f>Input!H12</f>
+        <f>Input!H13</f>
         <v>46500</v>
       </c>
       <c r="W6" s="68"/>
@@ -3232,7 +3245,7 @@
         <v>7</v>
       </c>
       <c r="AB6" s="151">
-        <f>Input!I12</f>
+        <f>Input!I13</f>
         <v>56000</v>
       </c>
       <c r="AC6" s="68"/>
@@ -3246,7 +3259,7 @@
         <v>7</v>
       </c>
       <c r="AH6" s="151">
-        <f>Input!J12</f>
+        <f>Input!J13</f>
         <v>56000</v>
       </c>
       <c r="AI6" s="68"/>
@@ -3266,7 +3279,7 @@
       <c r="H7" s="67"/>
       <c r="I7" s="58"/>
       <c r="J7" s="193">
-        <f>Input!F19</f>
+        <f>Input!F20</f>
         <v>23000</v>
       </c>
       <c r="K7" s="68"/>
@@ -3275,7 +3288,7 @@
       <c r="N7" s="67"/>
       <c r="O7" s="58"/>
       <c r="P7" s="193">
-        <f>Input!G19</f>
+        <f>Input!G20</f>
         <v>25000</v>
       </c>
       <c r="Q7" s="68"/>
@@ -3284,7 +3297,7 @@
       <c r="T7" s="67"/>
       <c r="U7" s="58"/>
       <c r="V7" s="193">
-        <f>Input!H19</f>
+        <f>Input!H20</f>
         <v>22500</v>
       </c>
       <c r="W7" s="68"/>
@@ -3293,7 +3306,7 @@
       <c r="Z7" s="67"/>
       <c r="AA7" s="58"/>
       <c r="AB7" s="152">
-        <f>Input!I19</f>
+        <f>Input!I20</f>
         <v>25600</v>
       </c>
       <c r="AC7" s="68"/>
@@ -3302,7 +3315,7 @@
       <c r="AF7" s="67"/>
       <c r="AG7" s="58"/>
       <c r="AH7" s="152">
-        <f>Input!J19</f>
+        <f>Input!J20</f>
         <v>25600</v>
       </c>
       <c r="AI7" s="68"/>
@@ -3527,14 +3540,14 @@
         <v>7</v>
       </c>
       <c r="J12" s="151">
-        <f>Input!F12</f>
+        <f>Input!F13</f>
         <v>45000</v>
       </c>
       <c r="K12" s="154" t="s">
         <v>26</v>
       </c>
       <c r="L12" s="151">
-        <f>Input!F17</f>
+        <f>Input!F18</f>
         <v>15000</v>
       </c>
       <c r="M12" s="85"/>
@@ -3546,14 +3559,14 @@
         <v>7</v>
       </c>
       <c r="P12" s="151">
-        <f>Input!G12</f>
+        <f>Input!G13</f>
         <v>46000</v>
       </c>
       <c r="Q12" s="154" t="s">
         <v>26</v>
       </c>
       <c r="R12" s="151">
-        <f>Input!G17</f>
+        <f>Input!G18</f>
         <v>18000</v>
       </c>
       <c r="S12" s="85"/>
@@ -3565,14 +3578,14 @@
         <v>7</v>
       </c>
       <c r="V12" s="151">
-        <f>Input!H12</f>
+        <f>Input!H13</f>
         <v>46500</v>
       </c>
       <c r="W12" s="154" t="s">
         <v>26</v>
       </c>
       <c r="X12" s="151">
-        <f>Input!H17</f>
+        <f>Input!H18</f>
         <v>16500</v>
       </c>
       <c r="Y12" s="85"/>
@@ -3584,14 +3597,14 @@
         <v>7</v>
       </c>
       <c r="AB12" s="151">
-        <f>Input!I12</f>
+        <f>Input!I13</f>
         <v>56000</v>
       </c>
       <c r="AC12" s="154" t="s">
         <v>26</v>
       </c>
       <c r="AD12" s="151">
-        <f>Input!I17</f>
+        <f>Input!I18</f>
         <v>14350</v>
       </c>
       <c r="AE12" s="85"/>
@@ -3603,14 +3616,14 @@
         <v>7</v>
       </c>
       <c r="AH12" s="151">
-        <f>Input!J12</f>
+        <f>Input!J13</f>
         <v>56000</v>
       </c>
       <c r="AI12" s="154" t="s">
         <v>26</v>
       </c>
       <c r="AJ12" s="151">
-        <f>Input!J17</f>
+        <f>Input!J18</f>
         <v>14350</v>
       </c>
       <c r="AK12" s="6"/>
@@ -3627,48 +3640,48 @@
       <c r="G13" s="66"/>
       <c r="H13" s="67"/>
       <c r="I13" s="58"/>
-      <c r="J13" s="201">
-        <f>Input!F19</f>
+      <c r="J13" s="199">
+        <f>Input!F20</f>
         <v>23000</v>
       </c>
-      <c r="K13" s="202"/>
-      <c r="L13" s="202"/>
+      <c r="K13" s="200"/>
+      <c r="L13" s="200"/>
       <c r="M13" s="86"/>
       <c r="N13" s="67"/>
       <c r="O13" s="58"/>
-      <c r="P13" s="201">
-        <f>Input!G19</f>
+      <c r="P13" s="199">
+        <f>Input!G20</f>
         <v>25000</v>
       </c>
-      <c r="Q13" s="202"/>
-      <c r="R13" s="202"/>
+      <c r="Q13" s="200"/>
+      <c r="R13" s="200"/>
       <c r="S13" s="86"/>
       <c r="T13" s="67"/>
       <c r="U13" s="58"/>
-      <c r="V13" s="201">
-        <f>Input!H19</f>
+      <c r="V13" s="199">
+        <f>Input!H20</f>
         <v>22500</v>
       </c>
-      <c r="W13" s="202"/>
-      <c r="X13" s="202"/>
+      <c r="W13" s="200"/>
+      <c r="X13" s="200"/>
       <c r="Y13" s="86"/>
       <c r="Z13" s="67"/>
       <c r="AA13" s="58"/>
-      <c r="AB13" s="201">
-        <f>Input!I19</f>
+      <c r="AB13" s="199">
+        <f>Input!I20</f>
         <v>25600</v>
       </c>
-      <c r="AC13" s="202"/>
-      <c r="AD13" s="202"/>
+      <c r="AC13" s="200"/>
+      <c r="AD13" s="200"/>
       <c r="AE13" s="86"/>
       <c r="AF13" s="67"/>
       <c r="AG13" s="58"/>
-      <c r="AH13" s="201">
-        <f>Input!J19</f>
+      <c r="AH13" s="199">
+        <f>Input!J20</f>
         <v>25600</v>
       </c>
-      <c r="AI13" s="202"/>
-      <c r="AJ13" s="202"/>
+      <c r="AI13" s="200"/>
+      <c r="AJ13" s="200"/>
       <c r="AK13" s="6"/>
     </row>
     <row r="14" spans="1:37">
@@ -3889,14 +3902,14 @@
         <v>7</v>
       </c>
       <c r="J18" s="151">
-        <f>Input!F12</f>
+        <f>Input!F13</f>
         <v>45000</v>
       </c>
       <c r="K18" s="154" t="s">
         <v>26</v>
       </c>
       <c r="L18" s="154">
-        <f>Input!F19</f>
+        <f>Input!F20</f>
         <v>23000</v>
       </c>
       <c r="M18" s="85"/>
@@ -3908,14 +3921,14 @@
         <v>7</v>
       </c>
       <c r="P18" s="151">
-        <f>Input!G12</f>
+        <f>Input!G13</f>
         <v>46000</v>
       </c>
       <c r="Q18" s="154" t="s">
         <v>26</v>
       </c>
       <c r="R18" s="154">
-        <f>Input!G19</f>
+        <f>Input!G20</f>
         <v>25000</v>
       </c>
       <c r="S18" s="85"/>
@@ -3927,14 +3940,14 @@
         <v>7</v>
       </c>
       <c r="V18" s="151">
-        <f>Input!H12</f>
+        <f>Input!H13</f>
         <v>46500</v>
       </c>
       <c r="W18" s="154" t="s">
         <v>26</v>
       </c>
       <c r="X18" s="154">
-        <f>Input!H19</f>
+        <f>Input!H20</f>
         <v>22500</v>
       </c>
       <c r="Y18" s="85"/>
@@ -3946,14 +3959,14 @@
         <v>7</v>
       </c>
       <c r="AB18" s="151">
-        <f>Input!I12</f>
+        <f>Input!I13</f>
         <v>56000</v>
       </c>
       <c r="AC18" s="154" t="s">
         <v>26</v>
       </c>
       <c r="AD18" s="154">
-        <f>Input!I19</f>
+        <f>Input!I20</f>
         <v>25600</v>
       </c>
       <c r="AE18" s="85"/>
@@ -3965,14 +3978,14 @@
         <v>7</v>
       </c>
       <c r="AH18" s="151">
-        <f>Input!J12</f>
+        <f>Input!J13</f>
         <v>56000</v>
       </c>
       <c r="AI18" s="154" t="s">
         <v>26</v>
       </c>
       <c r="AJ18" s="154">
-        <f>Input!J19</f>
+        <f>Input!J20</f>
         <v>25600</v>
       </c>
       <c r="AK18" s="6"/>
@@ -3989,48 +4002,48 @@
       <c r="G19" s="66"/>
       <c r="H19" s="67"/>
       <c r="I19" s="58"/>
-      <c r="J19" s="201">
-        <f>Input!F14</f>
+      <c r="J19" s="199">
+        <f>Input!F15</f>
         <v>125000</v>
       </c>
-      <c r="K19" s="202"/>
-      <c r="L19" s="202"/>
+      <c r="K19" s="200"/>
+      <c r="L19" s="200"/>
       <c r="M19" s="86"/>
       <c r="N19" s="67"/>
       <c r="O19" s="58"/>
-      <c r="P19" s="201">
-        <f>Input!G14</f>
+      <c r="P19" s="199">
+        <f>Input!G15</f>
         <v>126000</v>
       </c>
-      <c r="Q19" s="202"/>
-      <c r="R19" s="202"/>
+      <c r="Q19" s="200"/>
+      <c r="R19" s="200"/>
       <c r="S19" s="86"/>
       <c r="T19" s="67"/>
       <c r="U19" s="58"/>
-      <c r="V19" s="201">
-        <f>Input!H14</f>
+      <c r="V19" s="199">
+        <f>Input!H15</f>
         <v>126500</v>
       </c>
-      <c r="W19" s="202"/>
-      <c r="X19" s="202"/>
+      <c r="W19" s="200"/>
+      <c r="X19" s="200"/>
       <c r="Y19" s="86"/>
       <c r="Z19" s="67"/>
       <c r="AA19" s="58"/>
-      <c r="AB19" s="201">
-        <f>Input!I14</f>
+      <c r="AB19" s="199">
+        <f>Input!I15</f>
         <v>136000</v>
       </c>
-      <c r="AC19" s="202"/>
-      <c r="AD19" s="202"/>
+      <c r="AC19" s="200"/>
+      <c r="AD19" s="200"/>
       <c r="AE19" s="86"/>
       <c r="AF19" s="150"/>
       <c r="AG19" s="58"/>
-      <c r="AH19" s="201">
-        <f>Input!J14</f>
+      <c r="AH19" s="199">
+        <f>Input!J15</f>
         <v>136000</v>
       </c>
-      <c r="AI19" s="202"/>
-      <c r="AJ19" s="202"/>
+      <c r="AI19" s="200"/>
+      <c r="AJ19" s="200"/>
       <c r="AK19" s="6"/>
     </row>
     <row r="20" spans="1:37">
@@ -4290,7 +4303,7 @@
         <v>7</v>
       </c>
       <c r="J25" s="151">
-        <f>Input!F19</f>
+        <f>Input!F20</f>
         <v>23000</v>
       </c>
       <c r="K25" s="68"/>
@@ -4304,7 +4317,7 @@
         <v>7</v>
       </c>
       <c r="P25" s="151">
-        <f>Input!G19</f>
+        <f>Input!G20</f>
         <v>25000</v>
       </c>
       <c r="Q25" s="68"/>
@@ -4318,7 +4331,7 @@
         <v>7</v>
       </c>
       <c r="V25" s="151">
-        <f>Input!H19</f>
+        <f>Input!H20</f>
         <v>22500</v>
       </c>
       <c r="W25" s="68"/>
@@ -4332,7 +4345,7 @@
         <v>7</v>
       </c>
       <c r="AB25" s="151">
-        <f>Input!I19</f>
+        <f>Input!I20</f>
         <v>25600</v>
       </c>
       <c r="AC25" s="68"/>
@@ -4346,7 +4359,7 @@
         <v>7</v>
       </c>
       <c r="AH25" s="151">
-        <f>Input!J19</f>
+        <f>Input!J20</f>
         <v>25600</v>
       </c>
       <c r="AI25" s="68"/>
@@ -4366,7 +4379,7 @@
       <c r="H26" s="67"/>
       <c r="I26" s="58"/>
       <c r="J26" s="152">
-        <f>Input!F17</f>
+        <f>Input!F18</f>
         <v>15000</v>
       </c>
       <c r="K26" s="68"/>
@@ -4375,7 +4388,7 @@
       <c r="N26" s="67"/>
       <c r="O26" s="58"/>
       <c r="P26" s="152">
-        <f>Input!G17</f>
+        <f>Input!G18</f>
         <v>18000</v>
       </c>
       <c r="Q26" s="68"/>
@@ -4384,7 +4397,7 @@
       <c r="T26" s="67"/>
       <c r="U26" s="58"/>
       <c r="V26" s="152">
-        <f>Input!H17</f>
+        <f>Input!H18</f>
         <v>16500</v>
       </c>
       <c r="W26" s="68"/>
@@ -4393,7 +4406,7 @@
       <c r="Z26" s="67"/>
       <c r="AA26" s="58"/>
       <c r="AB26" s="152">
-        <f>Input!I17</f>
+        <f>Input!I18</f>
         <v>14350</v>
       </c>
       <c r="AC26" s="68"/>
@@ -4402,7 +4415,7 @@
       <c r="AF26" s="67"/>
       <c r="AG26" s="58"/>
       <c r="AH26" s="152">
-        <f>Input!J17</f>
+        <f>Input!J18</f>
         <v>14350</v>
       </c>
       <c r="AI26" s="68"/>
@@ -4666,7 +4679,7 @@
         <v>7</v>
       </c>
       <c r="J32" s="151">
-        <f>Input!F16</f>
+        <f>Input!F17</f>
         <v>15000</v>
       </c>
       <c r="K32" s="68"/>
@@ -4680,7 +4693,7 @@
         <v>7</v>
       </c>
       <c r="P32" s="151">
-        <f>Input!G16</f>
+        <f>Input!G17</f>
         <v>18000</v>
       </c>
       <c r="Q32" s="68"/>
@@ -4694,7 +4707,7 @@
         <v>7</v>
       </c>
       <c r="V32" s="151">
-        <f>Input!H16</f>
+        <f>Input!H17</f>
         <v>16500</v>
       </c>
       <c r="W32" s="68"/>
@@ -4708,7 +4721,7 @@
         <v>7</v>
       </c>
       <c r="AB32" s="151">
-        <f>Input!I16</f>
+        <f>Input!I17</f>
         <v>14350</v>
       </c>
       <c r="AC32" s="68"/>
@@ -4722,7 +4735,7 @@
         <v>7</v>
       </c>
       <c r="AH32" s="151">
-        <f>Input!J16</f>
+        <f>Input!J17</f>
         <v>14350</v>
       </c>
       <c r="AI32" s="68"/>
@@ -4742,7 +4755,7 @@
       <c r="H33" s="67"/>
       <c r="I33" s="58"/>
       <c r="J33" s="152">
-        <f>Input!F19</f>
+        <f>Input!F20</f>
         <v>23000</v>
       </c>
       <c r="K33" s="68"/>
@@ -4751,7 +4764,7 @@
       <c r="N33" s="67"/>
       <c r="O33" s="58"/>
       <c r="P33" s="152">
-        <f>Input!G19</f>
+        <f>Input!G20</f>
         <v>25000</v>
       </c>
       <c r="Q33" s="68"/>
@@ -4760,7 +4773,7 @@
       <c r="T33" s="67"/>
       <c r="U33" s="58"/>
       <c r="V33" s="152">
-        <f>Input!H19</f>
+        <f>Input!H20</f>
         <v>22500</v>
       </c>
       <c r="W33" s="68"/>
@@ -4769,7 +4782,7 @@
       <c r="Z33" s="67"/>
       <c r="AA33" s="58"/>
       <c r="AB33" s="152">
-        <f>Input!I19</f>
+        <f>Input!I20</f>
         <v>25600</v>
       </c>
       <c r="AC33" s="68"/>
@@ -4778,7 +4791,7 @@
       <c r="AF33" s="67"/>
       <c r="AG33" s="58"/>
       <c r="AH33" s="152">
-        <f>Input!J19</f>
+        <f>Input!J20</f>
         <v>25600</v>
       </c>
       <c r="AI33" s="68"/>
@@ -5003,7 +5016,7 @@
         <v>7</v>
       </c>
       <c r="J38" s="151">
-        <f>Input!F31</f>
+        <f>Input!F32</f>
         <v>68000</v>
       </c>
       <c r="K38" s="68"/>
@@ -5017,7 +5030,7 @@
         <v>7</v>
       </c>
       <c r="P38" s="151">
-        <f>Input!G31</f>
+        <f>Input!G32</f>
         <v>68000</v>
       </c>
       <c r="Q38" s="68"/>
@@ -5031,7 +5044,7 @@
         <v>7</v>
       </c>
       <c r="V38" s="151">
-        <f>Input!H31</f>
+        <f>Input!H32</f>
         <v>68000</v>
       </c>
       <c r="W38" s="68"/>
@@ -5045,7 +5058,7 @@
         <v>7</v>
       </c>
       <c r="AB38" s="151">
-        <f>Input!I31</f>
+        <f>Input!I32</f>
         <v>68000</v>
       </c>
       <c r="AC38" s="68"/>
@@ -5059,7 +5072,7 @@
         <v>7</v>
       </c>
       <c r="AH38" s="151">
-        <f>Input!J31</f>
+        <f>Input!J32</f>
         <v>272000</v>
       </c>
       <c r="AI38" s="68"/>
@@ -5079,7 +5092,7 @@
       <c r="H39" s="67"/>
       <c r="I39" s="58"/>
       <c r="J39" s="152">
-        <f>Input!F32</f>
+        <f>Input!F33</f>
         <v>77000</v>
       </c>
       <c r="K39" s="68"/>
@@ -5088,7 +5101,7 @@
       <c r="N39" s="67"/>
       <c r="O39" s="58"/>
       <c r="P39" s="152">
-        <f>Input!G32</f>
+        <f>Input!G33</f>
         <v>88000</v>
       </c>
       <c r="Q39" s="68"/>
@@ -5097,7 +5110,7 @@
       <c r="T39" s="67"/>
       <c r="U39" s="58"/>
       <c r="V39" s="152">
-        <f>Input!H32</f>
+        <f>Input!H33</f>
         <v>67600</v>
       </c>
       <c r="W39" s="68"/>
@@ -5106,7 +5119,7 @@
       <c r="Z39" s="67"/>
       <c r="AA39" s="58"/>
       <c r="AB39" s="152">
-        <f>Input!I32</f>
+        <f>Input!I33</f>
         <v>57000</v>
       </c>
       <c r="AC39" s="68"/>
@@ -5115,7 +5128,7 @@
       <c r="AF39" s="67"/>
       <c r="AG39" s="58"/>
       <c r="AH39" s="152">
-        <f>Input!J32</f>
+        <f>Input!J33</f>
         <v>289600</v>
       </c>
       <c r="AI39" s="68"/>
@@ -5420,7 +5433,7 @@
         <v>7</v>
       </c>
       <c r="J46" s="151">
-        <f>Input!F33</f>
+        <f>Input!F34</f>
         <v>18000</v>
       </c>
       <c r="K46" s="68"/>
@@ -5434,7 +5447,7 @@
         <v>7</v>
       </c>
       <c r="P46" s="151">
-        <f>Input!G33</f>
+        <f>Input!G34</f>
         <v>18000</v>
       </c>
       <c r="Q46" s="68"/>
@@ -5448,7 +5461,7 @@
         <v>7</v>
       </c>
       <c r="V46" s="151">
-        <f>Input!H33</f>
+        <f>Input!H34</f>
         <v>18000</v>
       </c>
       <c r="W46" s="68"/>
@@ -5462,7 +5475,7 @@
         <v>7</v>
       </c>
       <c r="AB46" s="151">
-        <f>Input!I33</f>
+        <f>Input!I34</f>
         <v>18000</v>
       </c>
       <c r="AC46" s="68"/>
@@ -5476,7 +5489,7 @@
         <v>7</v>
       </c>
       <c r="AH46" s="151">
-        <f>Input!J33</f>
+        <f>Input!J34</f>
         <v>72000</v>
       </c>
       <c r="AI46" s="68"/>
@@ -5496,7 +5509,7 @@
       <c r="H47" s="67"/>
       <c r="I47" s="58"/>
       <c r="J47" s="152">
-        <f>Input!F30</f>
+        <f>Input!F31</f>
         <v>145000</v>
       </c>
       <c r="K47" s="68"/>
@@ -5505,7 +5518,7 @@
       <c r="N47" s="67"/>
       <c r="O47" s="58"/>
       <c r="P47" s="152">
-        <f>Input!G30</f>
+        <f>Input!G31</f>
         <v>156000</v>
       </c>
       <c r="Q47" s="68"/>
@@ -5514,7 +5527,7 @@
       <c r="T47" s="67"/>
       <c r="U47" s="58"/>
       <c r="V47" s="152">
-        <f>Input!H30</f>
+        <f>Input!H31</f>
         <v>135600</v>
       </c>
       <c r="W47" s="68"/>
@@ -5523,7 +5536,7 @@
       <c r="Z47" s="67"/>
       <c r="AA47" s="58"/>
       <c r="AB47" s="152">
-        <f>Input!I30</f>
+        <f>Input!I31</f>
         <v>125000</v>
       </c>
       <c r="AC47" s="68"/>
@@ -5532,7 +5545,7 @@
       <c r="AF47" s="67"/>
       <c r="AG47" s="58"/>
       <c r="AH47" s="152">
-        <f>Input!J30</f>
+        <f>Input!J31</f>
         <v>561600</v>
       </c>
       <c r="AI47" s="68"/>
@@ -5796,7 +5809,7 @@
         <v>7</v>
       </c>
       <c r="J53" s="151">
-        <f>Input!F34</f>
+        <f>Input!F35</f>
         <v>11000</v>
       </c>
       <c r="K53" s="68"/>
@@ -5810,7 +5823,7 @@
         <v>7</v>
       </c>
       <c r="P53" s="151">
-        <f>Input!G34</f>
+        <f>Input!G35</f>
         <v>11000</v>
       </c>
       <c r="Q53" s="68"/>
@@ -5824,7 +5837,7 @@
         <v>7</v>
       </c>
       <c r="V53" s="151">
-        <f>Input!H34</f>
+        <f>Input!H35</f>
         <v>11000</v>
       </c>
       <c r="W53" s="68"/>
@@ -5838,7 +5851,7 @@
         <v>7</v>
       </c>
       <c r="AB53" s="151">
-        <f>Input!I34</f>
+        <f>Input!I35</f>
         <v>11000</v>
       </c>
       <c r="AC53" s="68"/>
@@ -5852,7 +5865,7 @@
         <v>7</v>
       </c>
       <c r="AH53" s="151">
-        <f>Input!J34</f>
+        <f>Input!J35</f>
         <v>44000</v>
       </c>
       <c r="AI53" s="68"/>
@@ -5874,7 +5887,7 @@
       <c r="H54" s="67"/>
       <c r="I54" s="58"/>
       <c r="J54" s="152">
-        <f>Input!F30</f>
+        <f>Input!F31</f>
         <v>145000</v>
       </c>
       <c r="K54" s="68"/>
@@ -5883,7 +5896,7 @@
       <c r="N54" s="67"/>
       <c r="O54" s="58"/>
       <c r="P54" s="152">
-        <f>Input!G30</f>
+        <f>Input!G31</f>
         <v>156000</v>
       </c>
       <c r="Q54" s="68"/>
@@ -5892,7 +5905,7 @@
       <c r="T54" s="67"/>
       <c r="U54" s="58"/>
       <c r="V54" s="152">
-        <f>Input!H30</f>
+        <f>Input!H31</f>
         <v>135600</v>
       </c>
       <c r="W54" s="68"/>
@@ -5901,7 +5914,7 @@
       <c r="Z54" s="67"/>
       <c r="AA54" s="58"/>
       <c r="AB54" s="152">
-        <f>Input!I30</f>
+        <f>Input!I31</f>
         <v>125000</v>
       </c>
       <c r="AC54" s="68"/>
@@ -5910,7 +5923,7 @@
       <c r="AF54" s="67"/>
       <c r="AG54" s="58"/>
       <c r="AH54" s="152">
-        <f>Input!J30</f>
+        <f>Input!J31</f>
         <v>561600</v>
       </c>
       <c r="AI54" s="68"/>
@@ -6191,6 +6204,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="G3:L3"/>
+    <mergeCell ref="M3:R3"/>
+    <mergeCell ref="S3:X3"/>
+    <mergeCell ref="V13:X13"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C25:C26"/>
     <mergeCell ref="AH13:AJ13"/>
     <mergeCell ref="P19:R19"/>
     <mergeCell ref="Y3:AD3"/>
@@ -6199,16 +6222,6 @@
     <mergeCell ref="AB19:AD19"/>
     <mergeCell ref="AE3:AJ3"/>
     <mergeCell ref="AH19:AJ19"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="G3:L3"/>
-    <mergeCell ref="M3:R3"/>
-    <mergeCell ref="S3:X3"/>
-    <mergeCell ref="V13:X13"/>
-    <mergeCell ref="P13:R13"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -6444,7 +6457,7 @@
         <v>7</v>
       </c>
       <c r="J6" s="156">
-        <f>Input!F30</f>
+        <f>Input!F31</f>
         <v>145000</v>
       </c>
       <c r="K6" s="98"/>
@@ -6456,7 +6469,7 @@
         <v>7</v>
       </c>
       <c r="N6" s="156">
-        <f>Input!G30</f>
+        <f>Input!G31</f>
         <v>156000</v>
       </c>
       <c r="O6" s="98"/>
@@ -6468,7 +6481,7 @@
         <v>7</v>
       </c>
       <c r="R6" s="156">
-        <f>Input!H30</f>
+        <f>Input!H31</f>
         <v>135600</v>
       </c>
       <c r="S6" s="99"/>
@@ -6480,7 +6493,7 @@
         <v>7</v>
       </c>
       <c r="V6" s="156">
-        <f>Input!I30</f>
+        <f>Input!I31</f>
         <v>125000</v>
       </c>
       <c r="W6" s="99"/>
@@ -6492,7 +6505,7 @@
         <v>7</v>
       </c>
       <c r="Z6" s="156">
-        <f>Input!J30</f>
+        <f>Input!J31</f>
         <v>561600</v>
       </c>
       <c r="AA6" s="93"/>
@@ -6510,35 +6523,35 @@
       <c r="H7" s="96"/>
       <c r="I7" s="58"/>
       <c r="J7" s="157">
-        <f>Input!F18</f>
+        <f>Input!F19</f>
         <v>13750</v>
       </c>
       <c r="K7" s="98"/>
       <c r="L7" s="96"/>
       <c r="M7" s="58"/>
       <c r="N7" s="157">
-        <f>Input!G18</f>
+        <f>Input!G19</f>
         <v>15250</v>
       </c>
       <c r="O7" s="98"/>
       <c r="P7" s="96"/>
       <c r="Q7" s="58"/>
       <c r="R7" s="157">
-        <f>Input!H18</f>
+        <f>Input!H19</f>
         <v>14500</v>
       </c>
       <c r="S7" s="99"/>
       <c r="T7" s="96"/>
       <c r="U7" s="58"/>
       <c r="V7" s="157">
-        <f>Input!I18</f>
+        <f>Input!I19</f>
         <v>13425</v>
       </c>
       <c r="W7" s="99"/>
       <c r="X7" s="96"/>
       <c r="Y7" s="58"/>
       <c r="Z7" s="157">
-        <f>Input!J18</f>
+        <f>Input!J19</f>
         <v>13425</v>
       </c>
       <c r="AA7" s="93"/>
@@ -6750,7 +6763,7 @@
         <v>7</v>
       </c>
       <c r="J13" s="156">
-        <f>Input!F30</f>
+        <f>Input!F31</f>
         <v>145000</v>
       </c>
       <c r="K13" s="98"/>
@@ -6762,7 +6775,7 @@
         <v>7</v>
       </c>
       <c r="N13" s="156">
-        <f>Input!G30</f>
+        <f>Input!G31</f>
         <v>156000</v>
       </c>
       <c r="O13" s="98"/>
@@ -6774,7 +6787,7 @@
         <v>7</v>
       </c>
       <c r="R13" s="156">
-        <f>Input!H30</f>
+        <f>Input!H31</f>
         <v>135600</v>
       </c>
       <c r="S13" s="99"/>
@@ -6786,7 +6799,7 @@
         <v>7</v>
       </c>
       <c r="V13" s="156">
-        <f>Input!I30</f>
+        <f>Input!I31</f>
         <v>125000</v>
       </c>
       <c r="W13" s="99"/>
@@ -6798,7 +6811,7 @@
         <v>7</v>
       </c>
       <c r="Z13" s="156">
-        <f>Input!J30</f>
+        <f>Input!J31</f>
         <v>561600</v>
       </c>
       <c r="AA13" s="93"/>
@@ -6816,35 +6829,35 @@
       <c r="H14" s="96"/>
       <c r="I14" s="58"/>
       <c r="J14" s="157">
-        <f>Input!F13</f>
+        <f>Input!F14</f>
         <v>80000</v>
       </c>
       <c r="K14" s="98"/>
       <c r="L14" s="96"/>
       <c r="M14" s="58"/>
       <c r="N14" s="157">
-        <f>Input!G13</f>
+        <f>Input!G14</f>
         <v>80000</v>
       </c>
       <c r="O14" s="98"/>
       <c r="P14" s="96"/>
       <c r="Q14" s="58"/>
       <c r="R14" s="157">
-        <f>Input!H13</f>
+        <f>Input!H14</f>
         <v>80000</v>
       </c>
       <c r="S14" s="99"/>
       <c r="T14" s="96"/>
       <c r="U14" s="58"/>
       <c r="V14" s="157">
-        <f>Input!I13</f>
+        <f>Input!I14</f>
         <v>80000</v>
       </c>
       <c r="W14" s="99"/>
       <c r="X14" s="96"/>
       <c r="Y14" s="58"/>
       <c r="Z14" s="157">
-        <f>Input!J13</f>
+        <f>Input!J14</f>
         <v>80000</v>
       </c>
       <c r="AA14" s="93"/>
@@ -7056,7 +7069,7 @@
         <v>7</v>
       </c>
       <c r="J20" s="156">
-        <f>Input!F30</f>
+        <f>Input!F31</f>
         <v>145000</v>
       </c>
       <c r="K20" s="98"/>
@@ -7068,7 +7081,7 @@
         <v>7</v>
       </c>
       <c r="N20" s="156">
-        <f>Input!G30</f>
+        <f>Input!G31</f>
         <v>156000</v>
       </c>
       <c r="O20" s="98"/>
@@ -7080,7 +7093,7 @@
         <v>7</v>
       </c>
       <c r="R20" s="156">
-        <f>Input!H30</f>
+        <f>Input!H31</f>
         <v>135600</v>
       </c>
       <c r="S20" s="99"/>
@@ -7092,7 +7105,7 @@
         <v>7</v>
       </c>
       <c r="V20" s="156">
-        <f>Input!I30</f>
+        <f>Input!I31</f>
         <v>125000</v>
       </c>
       <c r="W20" s="99"/>
@@ -7104,7 +7117,7 @@
         <v>7</v>
       </c>
       <c r="Z20" s="156">
-        <f>Input!J30</f>
+        <f>Input!J31</f>
         <v>561600</v>
       </c>
       <c r="AA20" s="93"/>
@@ -7122,35 +7135,35 @@
       <c r="H21" s="96"/>
       <c r="I21" s="58"/>
       <c r="J21" s="157">
-        <f>Input!F14</f>
+        <f>Input!F15</f>
         <v>125000</v>
       </c>
       <c r="K21" s="98"/>
       <c r="L21" s="96"/>
       <c r="M21" s="58"/>
       <c r="N21" s="157">
-        <f>Input!G14</f>
+        <f>Input!G15</f>
         <v>126000</v>
       </c>
       <c r="O21" s="98"/>
       <c r="P21" s="96"/>
       <c r="Q21" s="58"/>
       <c r="R21" s="157">
-        <f>Input!H14</f>
+        <f>Input!H15</f>
         <v>126500</v>
       </c>
       <c r="S21" s="99"/>
       <c r="T21" s="96"/>
       <c r="U21" s="58"/>
       <c r="V21" s="157">
-        <f>Input!I14</f>
+        <f>Input!I15</f>
         <v>136000</v>
       </c>
       <c r="W21" s="99"/>
       <c r="X21" s="96"/>
       <c r="Y21" s="58"/>
       <c r="Z21" s="157">
-        <f>Input!J14</f>
+        <f>Input!J15</f>
         <v>136000</v>
       </c>
       <c r="AA21" s="93"/>
@@ -7333,7 +7346,7 @@
         <v>7</v>
       </c>
       <c r="J26" s="156">
-        <f>Input!F14</f>
+        <f>Input!F15</f>
         <v>125000</v>
       </c>
       <c r="K26" s="98"/>
@@ -7345,7 +7358,7 @@
         <v>7</v>
       </c>
       <c r="N26" s="156">
-        <f>Input!G14</f>
+        <f>Input!G15</f>
         <v>126000</v>
       </c>
       <c r="O26" s="98"/>
@@ -7357,7 +7370,7 @@
         <v>7</v>
       </c>
       <c r="R26" s="156">
-        <f>Input!H14</f>
+        <f>Input!H15</f>
         <v>126500</v>
       </c>
       <c r="S26" s="99"/>
@@ -7369,7 +7382,7 @@
         <v>7</v>
       </c>
       <c r="V26" s="156">
-        <f>Input!I14</f>
+        <f>Input!I15</f>
         <v>136000</v>
       </c>
       <c r="W26" s="99"/>
@@ -7381,7 +7394,7 @@
         <v>7</v>
       </c>
       <c r="Z26" s="156">
-        <f>Input!J14</f>
+        <f>Input!J15</f>
         <v>136000</v>
       </c>
       <c r="AA26" s="93"/>
@@ -7399,35 +7412,35 @@
       <c r="H27" s="96"/>
       <c r="I27" s="58"/>
       <c r="J27" s="157">
-        <f>Input!F21</f>
+        <f>Input!F22</f>
         <v>28000</v>
       </c>
       <c r="K27" s="98"/>
       <c r="L27" s="96"/>
       <c r="M27" s="58"/>
       <c r="N27" s="157">
-        <f>Input!G21</f>
+        <f>Input!G22</f>
         <v>30900</v>
       </c>
       <c r="O27" s="98"/>
       <c r="P27" s="96"/>
       <c r="Q27" s="58"/>
       <c r="R27" s="157">
-        <f>Input!H21</f>
+        <f>Input!H22</f>
         <v>32000</v>
       </c>
       <c r="S27" s="99"/>
       <c r="T27" s="96"/>
       <c r="U27" s="58"/>
       <c r="V27" s="157">
-        <f>Input!I21</f>
+        <f>Input!I22</f>
         <v>26000</v>
       </c>
       <c r="W27" s="99"/>
       <c r="X27" s="96"/>
       <c r="Y27" s="58"/>
       <c r="Z27" s="157">
-        <f>Input!J21</f>
+        <f>Input!J22</f>
         <v>26000</v>
       </c>
       <c r="AA27" s="93"/>
@@ -7954,7 +7967,7 @@
         <v>7</v>
       </c>
       <c r="J6" s="156">
-        <f>Input!F37</f>
+        <f>Input!F38</f>
         <v>89000</v>
       </c>
       <c r="K6" s="85"/>
@@ -7966,7 +7979,7 @@
         <v>7</v>
       </c>
       <c r="N6" s="156">
-        <f>Input!G37</f>
+        <f>Input!G38</f>
         <v>87000</v>
       </c>
       <c r="O6" s="85"/>
@@ -7978,7 +7991,7 @@
         <v>7</v>
       </c>
       <c r="R6" s="156">
-        <f>Input!H37</f>
+        <f>Input!H38</f>
         <v>95000</v>
       </c>
       <c r="S6" s="85"/>
@@ -7990,7 +8003,7 @@
         <v>7</v>
       </c>
       <c r="V6" s="156">
-        <f>Input!I37</f>
+        <f>Input!I38</f>
         <v>65000</v>
       </c>
       <c r="W6" s="85"/>
@@ -8002,7 +8015,7 @@
         <v>7</v>
       </c>
       <c r="Z6" s="156">
-        <f>Input!J37</f>
+        <f>Input!J38</f>
         <v>336000</v>
       </c>
       <c r="AA6" s="93"/>
@@ -8021,35 +8034,35 @@
       <c r="H7" s="96"/>
       <c r="I7" s="58"/>
       <c r="J7" s="157">
-        <f>Input!F15</f>
+        <f>Input!F16</f>
         <v>122500</v>
       </c>
       <c r="K7" s="85"/>
       <c r="L7" s="96"/>
       <c r="M7" s="58"/>
       <c r="N7" s="157">
-        <f>Input!G15</f>
+        <f>Input!G16</f>
         <v>123000</v>
       </c>
       <c r="O7" s="85"/>
       <c r="P7" s="96"/>
       <c r="Q7" s="58"/>
       <c r="R7" s="157">
-        <f>Input!H15</f>
+        <f>Input!H16</f>
         <v>123250</v>
       </c>
       <c r="S7" s="85"/>
       <c r="T7" s="96"/>
       <c r="U7" s="58"/>
       <c r="V7" s="157">
-        <f>Input!I15</f>
+        <f>Input!I16</f>
         <v>128000</v>
       </c>
       <c r="W7" s="85"/>
       <c r="X7" s="96"/>
       <c r="Y7" s="58"/>
       <c r="Z7" s="157">
-        <f>Input!J15</f>
+        <f>Input!J16</f>
         <v>128000</v>
       </c>
       <c r="AA7" s="93"/>
@@ -8237,7 +8250,7 @@
         <v>7</v>
       </c>
       <c r="J12" s="156">
-        <f>Input!F37</f>
+        <f>Input!F38</f>
         <v>89000</v>
       </c>
       <c r="K12" s="85"/>
@@ -8249,7 +8262,7 @@
         <v>7</v>
       </c>
       <c r="N12" s="156">
-        <f>Input!G37</f>
+        <f>Input!G38</f>
         <v>87000</v>
       </c>
       <c r="O12" s="85"/>
@@ -8261,7 +8274,7 @@
         <v>7</v>
       </c>
       <c r="R12" s="156">
-        <f>Input!H37</f>
+        <f>Input!H38</f>
         <v>95000</v>
       </c>
       <c r="S12" s="85"/>
@@ -8273,7 +8286,7 @@
         <v>7</v>
       </c>
       <c r="V12" s="156">
-        <f>Input!I37</f>
+        <f>Input!I38</f>
         <v>65000</v>
       </c>
       <c r="W12" s="85"/>
@@ -8285,7 +8298,7 @@
         <v>7</v>
       </c>
       <c r="Z12" s="156">
-        <f>Input!J37</f>
+        <f>Input!J38</f>
         <v>336000</v>
       </c>
       <c r="AA12" s="93"/>
@@ -8304,35 +8317,35 @@
       <c r="H13" s="96"/>
       <c r="I13" s="58"/>
       <c r="J13" s="157">
-        <f>Input!F24</f>
+        <f>Input!F25</f>
         <v>28500</v>
       </c>
       <c r="K13" s="85"/>
       <c r="L13" s="96"/>
       <c r="M13" s="58"/>
       <c r="N13" s="157">
-        <f>Input!G24</f>
+        <f>Input!G25</f>
         <v>29950</v>
       </c>
       <c r="O13" s="85"/>
       <c r="P13" s="96"/>
       <c r="Q13" s="58"/>
       <c r="R13" s="157">
-        <f>Input!H24</f>
+        <f>Input!H25</f>
         <v>30500</v>
       </c>
       <c r="S13" s="85"/>
       <c r="T13" s="96"/>
       <c r="U13" s="58"/>
       <c r="V13" s="157">
-        <f>Input!I24</f>
+        <f>Input!I25</f>
         <v>27500</v>
       </c>
       <c r="W13" s="85"/>
       <c r="X13" s="96"/>
       <c r="Y13" s="58"/>
       <c r="Z13" s="157">
-        <f>Input!J24</f>
+        <f>Input!J25</f>
         <v>27500</v>
       </c>
       <c r="AA13" s="93"/>
@@ -8520,7 +8533,7 @@
         <v>7</v>
       </c>
       <c r="J18" s="156">
-        <f>Input!F37</f>
+        <f>Input!F38</f>
         <v>89000</v>
       </c>
       <c r="K18" s="85"/>
@@ -8532,7 +8545,7 @@
         <v>7</v>
       </c>
       <c r="N18" s="156">
-        <f>Input!G37</f>
+        <f>Input!G38</f>
         <v>87000</v>
       </c>
       <c r="O18" s="85"/>
@@ -8544,7 +8557,7 @@
         <v>7</v>
       </c>
       <c r="R18" s="156">
-        <f>Input!H37</f>
+        <f>Input!H38</f>
         <v>95000</v>
       </c>
       <c r="S18" s="85"/>
@@ -8556,7 +8569,7 @@
         <v>7</v>
       </c>
       <c r="V18" s="156">
-        <f>Input!I37</f>
+        <f>Input!I38</f>
         <v>65000</v>
       </c>
       <c r="W18" s="85"/>
@@ -8568,7 +8581,7 @@
         <v>7</v>
       </c>
       <c r="Z18" s="156">
-        <f>Input!J37</f>
+        <f>Input!J38</f>
         <v>336000</v>
       </c>
       <c r="AA18" s="93"/>
@@ -8587,35 +8600,35 @@
       <c r="H19" s="96"/>
       <c r="I19" s="58"/>
       <c r="J19" s="157">
-        <f>Input!F30</f>
+        <f>Input!F31</f>
         <v>145000</v>
       </c>
       <c r="K19" s="85"/>
       <c r="L19" s="96"/>
       <c r="M19" s="58"/>
       <c r="N19" s="157">
-        <f>Input!G30</f>
+        <f>Input!G31</f>
         <v>156000</v>
       </c>
       <c r="O19" s="85"/>
       <c r="P19" s="96"/>
       <c r="Q19" s="58"/>
       <c r="R19" s="157">
-        <f>Input!H30</f>
+        <f>Input!H31</f>
         <v>135600</v>
       </c>
       <c r="S19" s="85"/>
       <c r="T19" s="96"/>
       <c r="U19" s="58"/>
       <c r="V19" s="157">
-        <f>Input!I30</f>
+        <f>Input!I31</f>
         <v>125000</v>
       </c>
       <c r="W19" s="85"/>
       <c r="X19" s="96"/>
       <c r="Y19" s="58"/>
       <c r="Z19" s="157">
-        <f>Input!J30</f>
+        <f>Input!J31</f>
         <v>561600</v>
       </c>
       <c r="AA19" s="93"/>
@@ -8803,7 +8816,7 @@
         <v>7</v>
       </c>
       <c r="J24" s="156">
-        <f>Input!F35</f>
+        <f>Input!F36</f>
         <v>132000</v>
       </c>
       <c r="K24" s="85"/>
@@ -8815,7 +8828,7 @@
         <v>7</v>
       </c>
       <c r="N24" s="156">
-        <f>Input!G35</f>
+        <f>Input!G36</f>
         <v>127000</v>
       </c>
       <c r="O24" s="85"/>
@@ -8827,7 +8840,7 @@
         <v>7</v>
       </c>
       <c r="R24" s="156">
-        <f>Input!H35</f>
+        <f>Input!H36</f>
         <v>114500</v>
       </c>
       <c r="S24" s="85"/>
@@ -8839,7 +8852,7 @@
         <v>7</v>
       </c>
       <c r="V24" s="156">
-        <f>Input!I35</f>
+        <f>Input!I36</f>
         <v>98000</v>
       </c>
       <c r="W24" s="85"/>
@@ -8851,7 +8864,7 @@
         <v>7</v>
       </c>
       <c r="Z24" s="156">
-        <f>Input!J35</f>
+        <f>Input!J36</f>
         <v>471500</v>
       </c>
       <c r="AA24" s="93"/>
@@ -8870,35 +8883,35 @@
       <c r="H25" s="96"/>
       <c r="I25" s="58"/>
       <c r="J25" s="157">
-        <f>Input!F14</f>
+        <f>Input!F15</f>
         <v>125000</v>
       </c>
       <c r="K25" s="85"/>
       <c r="L25" s="96"/>
       <c r="M25" s="58"/>
       <c r="N25" s="157">
-        <f>Input!G14</f>
+        <f>Input!G15</f>
         <v>126000</v>
       </c>
       <c r="O25" s="85"/>
       <c r="P25" s="96"/>
       <c r="Q25" s="58"/>
       <c r="R25" s="157">
-        <f>Input!H14</f>
+        <f>Input!H15</f>
         <v>126500</v>
       </c>
       <c r="S25" s="85"/>
       <c r="T25" s="96"/>
       <c r="U25" s="58"/>
       <c r="V25" s="157">
-        <f>Input!I14</f>
+        <f>Input!I15</f>
         <v>136000</v>
       </c>
       <c r="W25" s="85"/>
       <c r="X25" s="96"/>
       <c r="Y25" s="58"/>
       <c r="Z25" s="157">
-        <f>Input!J14</f>
+        <f>Input!J15</f>
         <v>136000</v>
       </c>
       <c r="AA25" s="93"/>
@@ -9116,7 +9129,7 @@
         <v>7</v>
       </c>
       <c r="J31" s="156">
-        <f>Input!F37</f>
+        <f>Input!F38</f>
         <v>89000</v>
       </c>
       <c r="K31" s="85"/>
@@ -9128,7 +9141,7 @@
         <v>7</v>
       </c>
       <c r="N31" s="156">
-        <f>Input!G37</f>
+        <f>Input!G38</f>
         <v>87000</v>
       </c>
       <c r="O31" s="85"/>
@@ -9140,7 +9153,7 @@
         <v>7</v>
       </c>
       <c r="R31" s="156">
-        <f>Input!H37</f>
+        <f>Input!H38</f>
         <v>95000</v>
       </c>
       <c r="S31" s="85"/>
@@ -9152,7 +9165,7 @@
         <v>7</v>
       </c>
       <c r="V31" s="156">
-        <f>Input!I37</f>
+        <f>Input!I38</f>
         <v>65000</v>
       </c>
       <c r="W31" s="85"/>
@@ -9164,7 +9177,7 @@
         <v>7</v>
       </c>
       <c r="Z31" s="156">
-        <f>Input!J37</f>
+        <f>Input!J38</f>
         <v>336000</v>
       </c>
       <c r="AA31" s="93"/>
@@ -9183,35 +9196,35 @@
       <c r="H32" s="96"/>
       <c r="I32" s="58"/>
       <c r="J32" s="157">
-        <f>Input!F23</f>
+        <f>Input!F24</f>
         <v>25000</v>
       </c>
       <c r="K32" s="85"/>
       <c r="L32" s="96"/>
       <c r="M32" s="58"/>
       <c r="N32" s="157">
-        <f>Input!G23</f>
+        <f>Input!G24</f>
         <v>25000</v>
       </c>
       <c r="O32" s="85"/>
       <c r="P32" s="96"/>
       <c r="Q32" s="58"/>
       <c r="R32" s="157">
-        <f>Input!H23</f>
+        <f>Input!H24</f>
         <v>25000</v>
       </c>
       <c r="S32" s="85"/>
       <c r="T32" s="96"/>
       <c r="U32" s="58"/>
       <c r="V32" s="157">
-        <f>Input!I23</f>
+        <f>Input!I24</f>
         <v>25000</v>
       </c>
       <c r="W32" s="85"/>
       <c r="X32" s="96"/>
       <c r="Y32" s="58"/>
       <c r="Z32" s="157">
-        <f>Input!J23</f>
+        <f>Input!J24</f>
         <v>25000</v>
       </c>
       <c r="AA32" s="93"/>
@@ -10246,7 +10259,7 @@
         <v>7</v>
       </c>
       <c r="J6" s="156">
-        <f>Input!F20</f>
+        <f>Input!F21</f>
         <v>125000</v>
       </c>
       <c r="K6" s="98"/>
@@ -10258,7 +10271,7 @@
         <v>7</v>
       </c>
       <c r="N6" s="158">
-        <f>Input!G20</f>
+        <f>Input!G21</f>
         <v>125000</v>
       </c>
       <c r="O6" s="58"/>
@@ -10270,7 +10283,7 @@
         <v>7</v>
       </c>
       <c r="R6" s="158">
-        <f>Input!H20</f>
+        <f>Input!H21</f>
         <v>125000</v>
       </c>
       <c r="S6" s="17"/>
@@ -10282,7 +10295,7 @@
         <v>7</v>
       </c>
       <c r="V6" s="158">
-        <f>Input!I20</f>
+        <f>Input!I21</f>
         <v>110000</v>
       </c>
       <c r="W6" s="17"/>
@@ -10294,7 +10307,7 @@
         <v>7</v>
       </c>
       <c r="Z6" s="158">
-        <f>Input!J20</f>
+        <f>Input!J21</f>
         <v>110000</v>
       </c>
       <c r="AA6" s="17"/>
@@ -10314,35 +10327,35 @@
       <c r="H7" s="96"/>
       <c r="I7" s="58"/>
       <c r="J7" s="157">
-        <f>Input!F14</f>
+        <f>Input!F15</f>
         <v>125000</v>
       </c>
       <c r="K7" s="98"/>
       <c r="L7" s="96"/>
       <c r="M7" s="58"/>
       <c r="N7" s="156">
-        <f>Input!G14</f>
+        <f>Input!G15</f>
         <v>126000</v>
       </c>
       <c r="O7" s="98"/>
       <c r="P7" s="96"/>
       <c r="Q7" s="58"/>
       <c r="R7" s="156">
-        <f>Input!H14</f>
+        <f>Input!H15</f>
         <v>126500</v>
       </c>
       <c r="S7" s="99"/>
       <c r="T7" s="96"/>
       <c r="U7" s="58"/>
       <c r="V7" s="156">
-        <f>Input!I14</f>
+        <f>Input!I15</f>
         <v>136000</v>
       </c>
       <c r="W7" s="99"/>
       <c r="X7" s="96"/>
       <c r="Y7" s="58"/>
       <c r="Z7" s="156">
-        <f>Input!J14</f>
+        <f>Input!J15</f>
         <v>136000</v>
       </c>
       <c r="AA7" s="93"/>
@@ -10535,7 +10548,7 @@
         <v>7</v>
       </c>
       <c r="J12" s="156">
-        <f>Input!F35</f>
+        <f>Input!F36</f>
         <v>132000</v>
       </c>
       <c r="K12" s="98"/>
@@ -10547,7 +10560,7 @@
         <v>7</v>
       </c>
       <c r="N12" s="156">
-        <f>Input!G35</f>
+        <f>Input!G36</f>
         <v>127000</v>
       </c>
       <c r="O12" s="98"/>
@@ -10559,7 +10572,7 @@
         <v>7</v>
       </c>
       <c r="R12" s="156">
-        <f>Input!H35</f>
+        <f>Input!H36</f>
         <v>114500</v>
       </c>
       <c r="S12" s="99"/>
@@ -10571,7 +10584,7 @@
         <v>7</v>
       </c>
       <c r="V12" s="156">
-        <f>Input!I35</f>
+        <f>Input!I36</f>
         <v>98000</v>
       </c>
       <c r="W12" s="99"/>
@@ -10583,7 +10596,7 @@
         <v>7</v>
       </c>
       <c r="Z12" s="156">
-        <f>Input!J35</f>
+        <f>Input!J36</f>
         <v>471500</v>
       </c>
       <c r="AA12" s="93"/>
@@ -10603,35 +10616,35 @@
       <c r="H13" s="96"/>
       <c r="I13" s="58"/>
       <c r="J13" s="157">
-        <f>Input!F36</f>
+        <f>Input!F37</f>
         <v>24000</v>
       </c>
       <c r="K13" s="98"/>
       <c r="L13" s="96"/>
       <c r="M13" s="58"/>
       <c r="N13" s="157">
-        <f>Input!G36</f>
+        <f>Input!G37</f>
         <v>24000</v>
       </c>
       <c r="O13" s="98"/>
       <c r="P13" s="96"/>
       <c r="Q13" s="58"/>
       <c r="R13" s="157">
-        <f>Input!H36</f>
+        <f>Input!H37</f>
         <v>24000</v>
       </c>
       <c r="S13" s="99"/>
       <c r="T13" s="96"/>
       <c r="U13" s="58"/>
       <c r="V13" s="157">
-        <f>Input!I36</f>
+        <f>Input!I37</f>
         <v>24000</v>
       </c>
       <c r="W13" s="99"/>
       <c r="X13" s="96"/>
       <c r="Y13" s="58"/>
       <c r="Z13" s="157">
-        <f>Input!J36</f>
+        <f>Input!J37</f>
         <v>96000</v>
       </c>
       <c r="AA13" s="93"/>
@@ -10855,7 +10868,7 @@
         <v>7</v>
       </c>
       <c r="J19" s="156">
-        <f>Input!F20</f>
+        <f>Input!F21</f>
         <v>125000</v>
       </c>
       <c r="K19" s="98"/>
@@ -10867,7 +10880,7 @@
         <v>7</v>
       </c>
       <c r="N19" s="156">
-        <f>Input!G20</f>
+        <f>Input!G21</f>
         <v>125000</v>
       </c>
       <c r="O19" s="98"/>
@@ -10879,7 +10892,7 @@
         <v>7</v>
       </c>
       <c r="R19" s="156">
-        <f>Input!H20</f>
+        <f>Input!H21</f>
         <v>125000</v>
       </c>
       <c r="S19" s="99"/>
@@ -10891,7 +10904,7 @@
         <v>7</v>
       </c>
       <c r="V19" s="156">
-        <f>Input!I20</f>
+        <f>Input!I21</f>
         <v>110000</v>
       </c>
       <c r="W19" s="99"/>
@@ -10903,7 +10916,7 @@
         <v>7</v>
       </c>
       <c r="Z19" s="156">
-        <f>Input!J20</f>
+        <f>Input!J21</f>
         <v>110000</v>
       </c>
       <c r="AA19" s="93"/>
@@ -10923,35 +10936,35 @@
       <c r="H20" s="96"/>
       <c r="I20" s="58"/>
       <c r="J20" s="157">
-        <f>Input!F21</f>
+        <f>Input!F22</f>
         <v>28000</v>
       </c>
       <c r="K20" s="98"/>
       <c r="L20" s="96"/>
       <c r="M20" s="58"/>
       <c r="N20" s="157">
-        <f>Input!G21</f>
+        <f>Input!G22</f>
         <v>30900</v>
       </c>
       <c r="O20" s="98"/>
       <c r="P20" s="96"/>
       <c r="Q20" s="58"/>
       <c r="R20" s="157">
-        <f>Input!H21</f>
+        <f>Input!H22</f>
         <v>32000</v>
       </c>
       <c r="S20" s="99"/>
       <c r="T20" s="96"/>
       <c r="U20" s="58"/>
       <c r="V20" s="157">
-        <f>Input!I21</f>
+        <f>Input!I22</f>
         <v>26000</v>
       </c>
       <c r="W20" s="99"/>
       <c r="X20" s="96"/>
       <c r="Y20" s="58"/>
       <c r="Z20" s="157">
-        <f>Input!J21</f>
+        <f>Input!J22</f>
         <v>26000</v>
       </c>
       <c r="AA20" s="93"/>
@@ -11144,7 +11157,7 @@
         <v>7</v>
       </c>
       <c r="J25" s="158">
-        <f>Input!F39</f>
+        <f>Input!F40</f>
         <v>25000</v>
       </c>
       <c r="K25" s="98"/>
@@ -11156,7 +11169,7 @@
         <v>7</v>
       </c>
       <c r="N25" s="158">
-        <f>Input!G39</f>
+        <f>Input!G40</f>
         <v>24000</v>
       </c>
       <c r="O25" s="98"/>
@@ -11168,7 +11181,7 @@
         <v>7</v>
       </c>
       <c r="R25" s="158">
-        <f>Input!H39</f>
+        <f>Input!H40</f>
         <v>23000</v>
       </c>
       <c r="S25" s="99"/>
@@ -11180,7 +11193,7 @@
         <v>7</v>
       </c>
       <c r="V25" s="158">
-        <f>Input!I39</f>
+        <f>Input!I40</f>
         <v>22000</v>
       </c>
       <c r="W25" s="99"/>
@@ -11192,7 +11205,7 @@
         <v>7</v>
       </c>
       <c r="Z25" s="158">
-        <f>Input!J39</f>
+        <f>Input!J40</f>
         <v>22000</v>
       </c>
       <c r="AA25" s="93"/>
@@ -11212,35 +11225,35 @@
       <c r="H26" s="96"/>
       <c r="I26" s="58"/>
       <c r="J26" s="156">
-        <f>Input!F40</f>
+        <f>Input!F41</f>
         <v>65000</v>
       </c>
       <c r="K26" s="98"/>
       <c r="L26" s="96"/>
       <c r="M26" s="58"/>
       <c r="N26" s="156">
-        <f>Input!G40</f>
+        <f>Input!G41</f>
         <v>65000</v>
       </c>
       <c r="O26" s="98"/>
       <c r="P26" s="96"/>
       <c r="Q26" s="58"/>
       <c r="R26" s="156">
-        <f>Input!H40</f>
+        <f>Input!H41</f>
         <v>65000</v>
       </c>
       <c r="S26" s="99"/>
       <c r="T26" s="96"/>
       <c r="U26" s="58"/>
       <c r="V26" s="156">
-        <f>Input!I40</f>
+        <f>Input!I41</f>
         <v>65000</v>
       </c>
       <c r="W26" s="99"/>
       <c r="X26" s="96"/>
       <c r="Y26" s="58"/>
       <c r="Z26" s="156">
-        <f>Input!J40</f>
+        <f>Input!J41</f>
         <v>65000</v>
       </c>
       <c r="AA26" s="93"/>
@@ -11840,7 +11853,7 @@
         <v>7</v>
       </c>
       <c r="J6" s="151">
-        <f>Input!F37</f>
+        <f>Input!F38</f>
         <v>89000</v>
       </c>
       <c r="K6" s="97"/>
@@ -11852,7 +11865,7 @@
         <v>7</v>
       </c>
       <c r="N6" s="154">
-        <f>Input!G37</f>
+        <f>Input!G38</f>
         <v>87000</v>
       </c>
       <c r="O6" s="58"/>
@@ -11864,7 +11877,7 @@
         <v>7</v>
       </c>
       <c r="R6" s="154">
-        <f>Input!H37</f>
+        <f>Input!H38</f>
         <v>95000</v>
       </c>
       <c r="S6" s="17"/>
@@ -11876,7 +11889,7 @@
         <v>7</v>
       </c>
       <c r="V6" s="154">
-        <f>Input!I37</f>
+        <f>Input!I38</f>
         <v>65000</v>
       </c>
       <c r="W6" s="17"/>
@@ -11888,7 +11901,7 @@
         <v>7</v>
       </c>
       <c r="Z6" s="154">
-        <f>Input!J37</f>
+        <f>Input!J38</f>
         <v>336000</v>
       </c>
       <c r="AA6" s="17"/>
@@ -11908,35 +11921,35 @@
       <c r="H7" s="67"/>
       <c r="I7" s="58"/>
       <c r="J7" s="160">
-        <f>Input!F23</f>
+        <f>Input!F24</f>
         <v>25000</v>
       </c>
       <c r="K7" s="97"/>
       <c r="L7" s="67"/>
       <c r="M7" s="58"/>
       <c r="N7" s="163">
-        <f>Input!G23</f>
+        <f>Input!G24</f>
         <v>25000</v>
       </c>
       <c r="O7" s="98"/>
       <c r="P7" s="67"/>
       <c r="Q7" s="58"/>
       <c r="R7" s="163">
-        <f>Input!H23</f>
+        <f>Input!H24</f>
         <v>25000</v>
       </c>
       <c r="S7" s="99"/>
       <c r="T7" s="67"/>
       <c r="U7" s="58"/>
       <c r="V7" s="163">
-        <f>Input!I23</f>
+        <f>Input!I24</f>
         <v>25000</v>
       </c>
       <c r="W7" s="99"/>
       <c r="X7" s="67"/>
       <c r="Y7" s="58"/>
       <c r="Z7" s="163">
-        <f>Input!J23</f>
+        <f>Input!J24</f>
         <v>25000</v>
       </c>
       <c r="AA7" s="93"/>
@@ -12148,7 +12161,7 @@
         <v>7</v>
       </c>
       <c r="J13" s="162">
-        <f>Input!F25</f>
+        <f>Input!F26</f>
         <v>10</v>
       </c>
       <c r="K13" s="98"/>
@@ -12160,7 +12173,7 @@
         <v>7</v>
       </c>
       <c r="N13" s="162">
-        <f>Input!G25</f>
+        <f>Input!G26</f>
         <v>10</v>
       </c>
       <c r="O13" s="98"/>
@@ -12172,7 +12185,7 @@
         <v>7</v>
       </c>
       <c r="R13" s="162">
-        <f>Input!H25</f>
+        <f>Input!H26</f>
         <v>10</v>
       </c>
       <c r="S13" s="99"/>
@@ -12184,7 +12197,7 @@
         <v>7</v>
       </c>
       <c r="V13" s="162">
-        <f>Input!I25</f>
+        <f>Input!I26</f>
         <v>10</v>
       </c>
       <c r="W13" s="99"/>
@@ -12196,7 +12209,7 @@
         <v>7</v>
       </c>
       <c r="Z13" s="162">
-        <f>Input!J25</f>
+        <f>Input!J26</f>
         <v>10</v>
       </c>
       <c r="AA13" s="93"/>
@@ -12425,7 +12438,7 @@
         <v>7</v>
       </c>
       <c r="J19" s="162">
-        <f>Input!F25</f>
+        <f>Input!F26</f>
         <v>10</v>
       </c>
       <c r="K19" s="98"/>
@@ -12437,7 +12450,7 @@
         <v>7</v>
       </c>
       <c r="N19" s="162">
-        <f>Input!G25</f>
+        <f>Input!G26</f>
         <v>10</v>
       </c>
       <c r="O19" s="98"/>
@@ -12449,7 +12462,7 @@
         <v>7</v>
       </c>
       <c r="R19" s="162">
-        <f>Input!H25</f>
+        <f>Input!H26</f>
         <v>10</v>
       </c>
       <c r="S19" s="99"/>
@@ -12461,7 +12474,7 @@
         <v>7</v>
       </c>
       <c r="V19" s="162">
-        <f>Input!I25</f>
+        <f>Input!I26</f>
         <v>10</v>
       </c>
       <c r="W19" s="99"/>
@@ -12473,7 +12486,7 @@
         <v>7</v>
       </c>
       <c r="Z19" s="162">
-        <f>Input!J25</f>
+        <f>Input!J26</f>
         <v>10</v>
       </c>
       <c r="AA19" s="93"/>
@@ -12491,35 +12504,35 @@
       <c r="H20" s="67"/>
       <c r="I20" s="58"/>
       <c r="J20" s="161">
-        <f>Input!F27</f>
+        <f>Input!F28</f>
         <v>7</v>
       </c>
       <c r="K20" s="98"/>
       <c r="L20" s="67"/>
       <c r="M20" s="58"/>
       <c r="N20" s="161">
-        <f>Input!G27</f>
+        <f>Input!G28</f>
         <v>7.44</v>
       </c>
       <c r="O20" s="98"/>
       <c r="P20" s="67"/>
       <c r="Q20" s="58"/>
       <c r="R20" s="161">
-        <f>Input!H27</f>
+        <f>Input!H28</f>
         <v>6.76</v>
       </c>
       <c r="S20" s="99"/>
       <c r="T20" s="67"/>
       <c r="U20" s="58"/>
       <c r="V20" s="161">
-        <f>Input!I27</f>
+        <f>Input!I28</f>
         <v>6.2</v>
       </c>
       <c r="W20" s="99"/>
       <c r="X20" s="67"/>
       <c r="Y20" s="58"/>
       <c r="Z20" s="161">
-        <f>Input!J27</f>
+        <f>Input!J28</f>
         <v>27.4</v>
       </c>
       <c r="AA20" s="93"/>
@@ -12731,7 +12744,7 @@
         <v>7</v>
       </c>
       <c r="J26" s="151">
-        <f>Input!F28</f>
+        <f>Input!F29</f>
         <v>5000</v>
       </c>
       <c r="K26" s="98"/>
@@ -12743,7 +12756,7 @@
         <v>7</v>
       </c>
       <c r="N26" s="154">
-        <f>Input!G28</f>
+        <f>Input!G29</f>
         <v>5000</v>
       </c>
       <c r="O26" s="58"/>
@@ -12755,7 +12768,7 @@
         <v>7</v>
       </c>
       <c r="R26" s="151">
-        <f>Input!H28</f>
+        <f>Input!H29</f>
         <v>5000</v>
       </c>
       <c r="S26" s="99"/>
@@ -12767,7 +12780,7 @@
         <v>7</v>
       </c>
       <c r="V26" s="151">
-        <f>Input!I28</f>
+        <f>Input!I29</f>
         <v>5000</v>
       </c>
       <c r="W26" s="99"/>
@@ -12779,7 +12792,7 @@
         <v>7</v>
       </c>
       <c r="Z26" s="151">
-        <f>Input!J28</f>
+        <f>Input!J29</f>
         <v>20000</v>
       </c>
       <c r="AA26" s="93"/>
@@ -12797,35 +12810,35 @@
       <c r="H27" s="67"/>
       <c r="I27" s="58"/>
       <c r="J27" s="152">
-        <f>Input!F37</f>
+        <f>Input!F38</f>
         <v>89000</v>
       </c>
       <c r="K27" s="98"/>
       <c r="L27" s="67"/>
       <c r="M27" s="58"/>
       <c r="N27" s="151">
-        <f>Input!G37</f>
+        <f>Input!G38</f>
         <v>87000</v>
       </c>
       <c r="O27" s="98"/>
       <c r="P27" s="67"/>
       <c r="Q27" s="58"/>
       <c r="R27" s="152">
-        <f>Input!H37</f>
+        <f>Input!H38</f>
         <v>95000</v>
       </c>
       <c r="S27" s="17"/>
       <c r="T27" s="67"/>
       <c r="U27" s="58"/>
       <c r="V27" s="152">
-        <f>Input!I37</f>
+        <f>Input!I38</f>
         <v>65000</v>
       </c>
       <c r="W27" s="99"/>
       <c r="X27" s="67"/>
       <c r="Y27" s="58"/>
       <c r="Z27" s="152">
-        <f>Input!J37</f>
+        <f>Input!J38</f>
         <v>336000</v>
       </c>
       <c r="AA27" s="93"/>

</xml_diff>